<commit_message>
Improvements to TestingScript_ALT. First draft of ValveTimingProcessFunc.
</commit_message>
<xml_diff>
--- a/Relief Valve Selector/ReliefValveSelectorReference.xlsx
+++ b/Relief Valve Selector/ReliefValveSelectorReference.xlsx
@@ -5,15 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AustinThomas\Desktop\MATLAB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AustinThomas\Desktop\MATLAB\MARS\Relief Valve Selector\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C0A06AC-CA0A-43B6-BB3E-E8529509D699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124FB887-AE68-46E2-99C5-D384DFCD2E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31980" yWindow="2025" windowWidth="21600" windowHeight="11325" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="CommodityRef" sheetId="1" r:id="rId1"/>
+    <sheet name="ModelTypeRef" sheetId="3" r:id="rId2"/>
+    <sheet name="ThermoRef" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
   <si>
     <t>Commodity</t>
   </si>
@@ -33,20 +35,158 @@
     <t>State</t>
   </si>
   <si>
-    <t>Molecular Weight</t>
-  </si>
-  <si>
-    <t>Specific Gravity</t>
-  </si>
-  <si>
-    <t>Gas Constant</t>
+    <t>SpecificGravity</t>
+  </si>
+  <si>
+    <t>MolecularWeight</t>
+  </si>
+  <si>
+    <t>GasConstant</t>
+  </si>
+  <si>
+    <t>GN2</t>
+  </si>
+  <si>
+    <t>gas</t>
+  </si>
+  <si>
+    <t>GHe</t>
+  </si>
+  <si>
+    <t>81P</t>
+  </si>
+  <si>
+    <t>63B</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>ValveType</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>-2</t>
+  </si>
+  <si>
+    <t>-4</t>
+  </si>
+  <si>
+    <t>-5</t>
+  </si>
+  <si>
+    <t>-6</t>
+  </si>
+  <si>
+    <t>-7</t>
+  </si>
+  <si>
+    <t>-8</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>T Max</t>
+  </si>
+  <si>
+    <t>T Min</t>
+  </si>
+  <si>
+    <t>-2 P Min</t>
+  </si>
+  <si>
+    <t>-2 P Max</t>
+  </si>
+  <si>
+    <t>-4 P Min</t>
+  </si>
+  <si>
+    <t>-4 P Max</t>
+  </si>
+  <si>
+    <t>-6 P Min</t>
+  </si>
+  <si>
+    <t>-5 P Max</t>
+  </si>
+  <si>
+    <t>-5 P Min</t>
+  </si>
+  <si>
+    <t>-6 P Max</t>
+  </si>
+  <si>
+    <t>-7 P Min</t>
+  </si>
+  <si>
+    <t>-7 P Max</t>
+  </si>
+  <si>
+    <t>-8 P Min</t>
+  </si>
+  <si>
+    <t>-8 P Max</t>
+  </si>
+  <si>
+    <t>-F P Min</t>
+  </si>
+  <si>
+    <t>-F P Max</t>
+  </si>
+  <si>
+    <t>-G P Min</t>
+  </si>
+  <si>
+    <t>-G P Max</t>
+  </si>
+  <si>
+    <t>-H P Min</t>
+  </si>
+  <si>
+    <t>-H P Max</t>
+  </si>
+  <si>
+    <t>-J P Min</t>
+  </si>
+  <si>
+    <t>- J P Max</t>
+  </si>
+  <si>
+    <t>Seat Material</t>
+  </si>
+  <si>
+    <t>NBR</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,8 +194,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -68,8 +216,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -77,13 +237,186 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -366,10 +699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -383,20 +716,543 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="D2" s="11">
+        <v>28.01</v>
+      </c>
+      <c r="E2" s="12">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="8">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D3" s="15">
+        <v>4</v>
+      </c>
+      <c r="E3" s="16">
+        <v>378</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA9D8965-069B-4667-A351-BA2CC7871A2D}">
+  <dimension ref="A1:L8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1.2E-2</v>
+      </c>
+      <c r="D2" s="2">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="E2" s="2">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0.11</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0.307</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0.503</v>
+      </c>
+      <c r="K2" s="2">
+        <v>0.78500000000000003</v>
+      </c>
+      <c r="L2" s="19">
+        <v>1.2869999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="17">
+        <v>81</v>
+      </c>
+      <c r="B3" s="7">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="C3" s="20">
+        <v>0</v>
+      </c>
+      <c r="D3" s="20">
+        <v>1</v>
+      </c>
+      <c r="E3" s="20">
+        <v>0</v>
+      </c>
+      <c r="F3" s="20">
+        <v>1</v>
+      </c>
+      <c r="G3" s="20">
+        <v>0</v>
+      </c>
+      <c r="H3" s="20">
+        <v>1</v>
+      </c>
+      <c r="I3" s="20">
+        <v>1</v>
+      </c>
+      <c r="J3" s="20">
+        <v>1</v>
+      </c>
+      <c r="K3" s="20">
+        <v>1</v>
+      </c>
+      <c r="L3" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.72</v>
+      </c>
+      <c r="C4" s="22">
+        <v>0</v>
+      </c>
+      <c r="D4" s="22">
+        <v>1</v>
+      </c>
+      <c r="E4" s="22">
+        <v>0</v>
+      </c>
+      <c r="F4" s="22">
+        <v>0</v>
+      </c>
+      <c r="G4" s="22">
+        <v>0</v>
+      </c>
+      <c r="H4" s="22">
+        <v>1</v>
+      </c>
+      <c r="I4" s="22">
+        <v>0</v>
+      </c>
+      <c r="J4" s="22">
+        <v>1</v>
+      </c>
+      <c r="K4" s="22">
+        <v>0</v>
+      </c>
+      <c r="L4" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="17">
+        <v>83</v>
+      </c>
+      <c r="B5" s="7">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="C5" s="20">
+        <v>0</v>
+      </c>
+      <c r="D5" s="20">
+        <v>1</v>
+      </c>
+      <c r="E5" s="20">
+        <v>0</v>
+      </c>
+      <c r="F5" s="20">
+        <v>1</v>
+      </c>
+      <c r="G5" s="20">
+        <v>0</v>
+      </c>
+      <c r="H5" s="20">
+        <v>1</v>
+      </c>
+      <c r="I5" s="20">
+        <v>1</v>
+      </c>
+      <c r="J5" s="20">
+        <v>1</v>
+      </c>
+      <c r="K5" s="20">
+        <v>1</v>
+      </c>
+      <c r="L5" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>84</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="C6" s="22">
+        <v>1</v>
+      </c>
+      <c r="D6" s="22">
+        <v>0</v>
+      </c>
+      <c r="E6" s="22">
+        <v>0</v>
+      </c>
+      <c r="F6" s="22">
+        <v>0</v>
+      </c>
+      <c r="G6" s="22">
+        <v>0</v>
+      </c>
+      <c r="H6" s="22">
+        <v>0</v>
+      </c>
+      <c r="I6" s="22">
+        <v>0</v>
+      </c>
+      <c r="J6" s="22">
+        <v>0</v>
+      </c>
+      <c r="K6" s="22">
+        <v>0</v>
+      </c>
+      <c r="L6" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="7">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="C7" s="20">
+        <v>0</v>
+      </c>
+      <c r="D7" s="20">
+        <v>0</v>
+      </c>
+      <c r="E7" s="20">
+        <v>1</v>
+      </c>
+      <c r="F7" s="20">
+        <v>0</v>
+      </c>
+      <c r="G7" s="20">
+        <v>0</v>
+      </c>
+      <c r="H7" s="20">
+        <v>0</v>
+      </c>
+      <c r="I7" s="20">
+        <v>0</v>
+      </c>
+      <c r="J7" s="20">
+        <v>0</v>
+      </c>
+      <c r="K7" s="20">
+        <v>0</v>
+      </c>
+      <c r="L7" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.86099999999999999</v>
+      </c>
+      <c r="C8" s="23">
+        <v>0</v>
+      </c>
+      <c r="D8" s="23">
+        <v>0</v>
+      </c>
+      <c r="E8" s="23">
+        <v>0</v>
+      </c>
+      <c r="F8" s="23">
+        <v>0</v>
+      </c>
+      <c r="G8" s="23">
+        <v>1</v>
+      </c>
+      <c r="H8" s="23">
+        <v>0</v>
+      </c>
+      <c r="I8" s="23">
+        <v>0</v>
+      </c>
+      <c r="J8" s="23">
+        <v>0</v>
+      </c>
+      <c r="K8" s="23">
+        <v>0</v>
+      </c>
+      <c r="L8" s="24">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B5E9472-F4F9-472D-A559-24D5CE8770E9}">
+  <dimension ref="A1:AA14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="14.5703125" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q1" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="R1" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="S1" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="T1" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="U1" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="V1" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="W1" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="X1" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y1" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z1" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA1" s="29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>83</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="1">
+        <v>-65</v>
+      </c>
+      <c r="E2" s="1">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="J14" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Major changes to relief valve selector function and associated reference .xlsx; WIP
</commit_message>
<xml_diff>
--- a/Relief Valve Selector/ReliefValveSelectorReference.xlsx
+++ b/Relief Valve Selector/ReliefValveSelectorReference.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AustinThomas\Desktop\MATLAB\MARS\Relief Valve Selector\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124FB887-AE68-46E2-99C5-D384DFCD2E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDEA375B-839A-47CD-A1D4-50A7EB4385B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31980" yWindow="2025" windowWidth="21600" windowHeight="11325" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="CommodityRef" sheetId="1" r:id="rId1"/>
-    <sheet name="ModelTypeRef" sheetId="3" r:id="rId2"/>
-    <sheet name="ThermoRef" sheetId="4" r:id="rId3"/>
+    <sheet name="Master" sheetId="7" r:id="rId1"/>
+    <sheet name="CommodityRef" sheetId="1" r:id="rId2"/>
+    <sheet name="ModelTypeRef" sheetId="3" r:id="rId3"/>
+    <sheet name="ThermoSeatRef" sheetId="4" r:id="rId4"/>
+    <sheet name="TempMaterialRef" sheetId="5" r:id="rId5"/>
+    <sheet name="SeatAndMatRef" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="97">
   <si>
     <t>Commodity</t>
   </si>
@@ -86,84 +89,24 @@
     <t>-8</t>
   </si>
   <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>J</t>
-  </si>
-  <si>
     <t>T Max</t>
   </si>
   <si>
     <t>T Min</t>
   </si>
   <si>
-    <t>-2 P Min</t>
-  </si>
-  <si>
-    <t>-2 P Max</t>
-  </si>
-  <si>
-    <t>-4 P Min</t>
-  </si>
-  <si>
-    <t>-4 P Max</t>
-  </si>
-  <si>
-    <t>-6 P Min</t>
-  </si>
-  <si>
     <t>-5 P Max</t>
   </si>
   <si>
     <t>-5 P Min</t>
   </si>
   <si>
-    <t>-6 P Max</t>
-  </si>
-  <si>
     <t>-7 P Min</t>
   </si>
   <si>
     <t>-7 P Max</t>
   </si>
   <si>
-    <t>-8 P Min</t>
-  </si>
-  <si>
-    <t>-8 P Max</t>
-  </si>
-  <si>
-    <t>-F P Min</t>
-  </si>
-  <si>
-    <t>-F P Max</t>
-  </si>
-  <si>
-    <t>-G P Min</t>
-  </si>
-  <si>
-    <t>-G P Max</t>
-  </si>
-  <si>
-    <t>-H P Min</t>
-  </si>
-  <si>
-    <t>-H P Max</t>
-  </si>
-  <si>
-    <t>-J P Min</t>
-  </si>
-  <si>
-    <t>- J P Max</t>
-  </si>
-  <si>
     <t>Seat Material</t>
   </si>
   <si>
@@ -177,6 +120,207 @@
   </si>
   <si>
     <t xml:space="preserve">      </t>
+  </si>
+  <si>
+    <t>FKM</t>
+  </si>
+  <si>
+    <t>EPR</t>
+  </si>
+  <si>
+    <t>FFKM</t>
+  </si>
+  <si>
+    <t>PTFE</t>
+  </si>
+  <si>
+    <t>PCTFE</t>
+  </si>
+  <si>
+    <t>Vespel</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>Brass</t>
+  </si>
+  <si>
+    <t>CD</t>
+  </si>
+  <si>
+    <t>Arlon 300 XT</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>-F</t>
+  </si>
+  <si>
+    <t>-G</t>
+  </si>
+  <si>
+    <t>-H</t>
+  </si>
+  <si>
+    <t>-J</t>
+  </si>
+  <si>
+    <t>-2 P Min (SS)</t>
+  </si>
+  <si>
+    <t>-2 P Max (SS)</t>
+  </si>
+  <si>
+    <t>-4 P Min (Brass)</t>
+  </si>
+  <si>
+    <t>-4 P Max (Brass)</t>
+  </si>
+  <si>
+    <t>-4 P Min (CS/SS)</t>
+  </si>
+  <si>
+    <t>-4 P Max (CS/SS)</t>
+  </si>
+  <si>
+    <t>-6 P Min (Brass)</t>
+  </si>
+  <si>
+    <t>-6 P Max (Brass)</t>
+  </si>
+  <si>
+    <t>-6 P Min (CS/SS)</t>
+  </si>
+  <si>
+    <t>-6 P Max (CS/SS)</t>
+  </si>
+  <si>
+    <t>-8 P Min (Brass)</t>
+  </si>
+  <si>
+    <t>-8 P Max (Brass)</t>
+  </si>
+  <si>
+    <t>-F P Min (CS/SS)</t>
+  </si>
+  <si>
+    <t>-8 P Min (CS/SS)</t>
+  </si>
+  <si>
+    <t>-8 P Max (CS/SS)</t>
+  </si>
+  <si>
+    <t>-F P Min (Brass)</t>
+  </si>
+  <si>
+    <t>-F P Max (Brass)</t>
+  </si>
+  <si>
+    <t>-G P Min (Brass)</t>
+  </si>
+  <si>
+    <t>-G P Max (Brass)</t>
+  </si>
+  <si>
+    <t>-H P Min (Brass)</t>
+  </si>
+  <si>
+    <t>-H P Max (Brass)</t>
+  </si>
+  <si>
+    <t>-J P Min (Brass)</t>
+  </si>
+  <si>
+    <t>- J P Max (Brass)</t>
+  </si>
+  <si>
+    <t>-F P Max (CS/SS)</t>
+  </si>
+  <si>
+    <t>-G P Min (CS/SS)</t>
+  </si>
+  <si>
+    <t>-G P Max (CS/SS)</t>
+  </si>
+  <si>
+    <t>-H P Min (CS/SS)</t>
+  </si>
+  <si>
+    <t>-H P Max (CS/SS)</t>
+  </si>
+  <si>
+    <t>-J P Min (CS/SS)</t>
+  </si>
+  <si>
+    <t>- J P Max (CS/SS)</t>
+  </si>
+  <si>
+    <t>-2 (SS)</t>
+  </si>
+  <si>
+    <t>-4 (Brass)</t>
+  </si>
+  <si>
+    <t>-4 (CS)</t>
+  </si>
+  <si>
+    <t>-4 (SS)</t>
+  </si>
+  <si>
+    <t>-6 (Brass)</t>
+  </si>
+  <si>
+    <t>-6 (CS)</t>
+  </si>
+  <si>
+    <t>-6 (SS)</t>
+  </si>
+  <si>
+    <t>-8 (Brass)</t>
+  </si>
+  <si>
+    <t>-8 (CS)</t>
+  </si>
+  <si>
+    <t>-8 (SS)</t>
+  </si>
+  <si>
+    <t>-F (Brass)</t>
+  </si>
+  <si>
+    <t>-F (CS)</t>
+  </si>
+  <si>
+    <t>-F (SS)</t>
+  </si>
+  <si>
+    <t>-G (Brass)</t>
+  </si>
+  <si>
+    <t>-G (CS)</t>
+  </si>
+  <si>
+    <t>-G (SS)</t>
+  </si>
+  <si>
+    <t>-H (Brass)</t>
+  </si>
+  <si>
+    <t>-H (CS)</t>
+  </si>
+  <si>
+    <t>-H (SS)</t>
+  </si>
+  <si>
+    <t>-J (Brass)</t>
+  </si>
+  <si>
+    <t>-J (CS)</t>
+  </si>
+  <si>
+    <t>-J (SS)</t>
   </si>
 </sst>
 </file>
@@ -327,7 +471,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -416,7 +560,40 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -698,6 +875,1147 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C12848D-D482-4AD5-8ACF-BF2FE2CFA96B}">
+  <dimension ref="A1:Z14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X25" sqref="X25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="1" customWidth="1"/>
+    <col min="3" max="26" width="10.7109375" style="1" customWidth="1"/>
+    <col min="27" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="J1" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="M1" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="N1" s="40" t="s">
+        <v>84</v>
+      </c>
+      <c r="O1" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="P1" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q1" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="R1" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="S1" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="T1" s="40" t="s">
+        <v>90</v>
+      </c>
+      <c r="U1" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="V1" s="40" t="s">
+        <v>92</v>
+      </c>
+      <c r="W1" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="X1" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y1" s="40" t="s">
+        <v>95</v>
+      </c>
+      <c r="Z1" s="41" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2" s="30">
+        <v>83</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="31">
+        <v>0</v>
+      </c>
+      <c r="D2" s="31">
+        <v>0</v>
+      </c>
+      <c r="E2" s="31">
+        <v>0</v>
+      </c>
+      <c r="F2" s="31">
+        <v>0</v>
+      </c>
+      <c r="G2" s="31">
+        <v>0</v>
+      </c>
+      <c r="H2" s="31">
+        <v>0</v>
+      </c>
+      <c r="I2" s="31">
+        <v>0</v>
+      </c>
+      <c r="J2" s="31">
+        <v>0</v>
+      </c>
+      <c r="K2" s="31">
+        <v>0</v>
+      </c>
+      <c r="L2" s="31">
+        <v>0</v>
+      </c>
+      <c r="M2" s="31">
+        <v>0</v>
+      </c>
+      <c r="N2" s="31">
+        <v>0</v>
+      </c>
+      <c r="O2" s="31">
+        <v>0</v>
+      </c>
+      <c r="P2" s="31">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="31">
+        <v>0</v>
+      </c>
+      <c r="R2" s="31">
+        <v>0</v>
+      </c>
+      <c r="S2" s="31">
+        <v>0</v>
+      </c>
+      <c r="T2" s="31">
+        <v>0</v>
+      </c>
+      <c r="U2" s="31">
+        <v>0</v>
+      </c>
+      <c r="V2" s="31">
+        <v>0</v>
+      </c>
+      <c r="W2" s="31">
+        <v>0</v>
+      </c>
+      <c r="X2" s="31">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="31">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3" s="36">
+        <v>83</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="37">
+        <v>0</v>
+      </c>
+      <c r="D3" s="37">
+        <v>0</v>
+      </c>
+      <c r="E3" s="37">
+        <v>0</v>
+      </c>
+      <c r="F3" s="37">
+        <v>0</v>
+      </c>
+      <c r="G3" s="37">
+        <v>0</v>
+      </c>
+      <c r="H3" s="37">
+        <v>0</v>
+      </c>
+      <c r="I3" s="37">
+        <v>0</v>
+      </c>
+      <c r="J3" s="37">
+        <v>0</v>
+      </c>
+      <c r="K3" s="37">
+        <v>0</v>
+      </c>
+      <c r="L3" s="37">
+        <v>0</v>
+      </c>
+      <c r="M3" s="37">
+        <v>0</v>
+      </c>
+      <c r="N3" s="37">
+        <v>0</v>
+      </c>
+      <c r="O3" s="37">
+        <v>0</v>
+      </c>
+      <c r="P3" s="37">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="37">
+        <v>0</v>
+      </c>
+      <c r="R3" s="37">
+        <v>0</v>
+      </c>
+      <c r="S3" s="37">
+        <v>0</v>
+      </c>
+      <c r="T3" s="37">
+        <v>0</v>
+      </c>
+      <c r="U3" s="37">
+        <v>0</v>
+      </c>
+      <c r="V3" s="37">
+        <v>0</v>
+      </c>
+      <c r="W3" s="37">
+        <v>0</v>
+      </c>
+      <c r="X3" s="37">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="37">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4" s="30">
+        <v>83</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="31">
+        <v>0</v>
+      </c>
+      <c r="D4" s="31">
+        <v>0</v>
+      </c>
+      <c r="E4" s="31">
+        <v>0</v>
+      </c>
+      <c r="F4" s="31">
+        <v>0</v>
+      </c>
+      <c r="G4" s="31">
+        <v>0</v>
+      </c>
+      <c r="H4" s="31">
+        <v>0</v>
+      </c>
+      <c r="I4" s="31">
+        <v>0</v>
+      </c>
+      <c r="J4" s="31">
+        <v>0</v>
+      </c>
+      <c r="K4" s="31">
+        <v>0</v>
+      </c>
+      <c r="L4" s="31">
+        <v>0</v>
+      </c>
+      <c r="M4" s="31">
+        <v>0</v>
+      </c>
+      <c r="N4" s="31">
+        <v>0</v>
+      </c>
+      <c r="O4" s="31">
+        <v>0</v>
+      </c>
+      <c r="P4" s="31">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="31">
+        <v>0</v>
+      </c>
+      <c r="R4" s="31">
+        <v>0</v>
+      </c>
+      <c r="S4" s="31">
+        <v>0</v>
+      </c>
+      <c r="T4" s="31">
+        <v>0</v>
+      </c>
+      <c r="U4" s="31">
+        <v>0</v>
+      </c>
+      <c r="V4" s="31">
+        <v>0</v>
+      </c>
+      <c r="W4" s="31">
+        <v>0</v>
+      </c>
+      <c r="X4" s="31">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="31">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5" s="36">
+        <v>83</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="37">
+        <v>0</v>
+      </c>
+      <c r="D5" s="37">
+        <v>0</v>
+      </c>
+      <c r="E5" s="37">
+        <v>0</v>
+      </c>
+      <c r="F5" s="37">
+        <v>0</v>
+      </c>
+      <c r="G5" s="37">
+        <v>0</v>
+      </c>
+      <c r="H5" s="37">
+        <v>0</v>
+      </c>
+      <c r="I5" s="37">
+        <v>0</v>
+      </c>
+      <c r="J5" s="37">
+        <v>0</v>
+      </c>
+      <c r="K5" s="37">
+        <v>0</v>
+      </c>
+      <c r="L5" s="37">
+        <v>0</v>
+      </c>
+      <c r="M5" s="37">
+        <v>0</v>
+      </c>
+      <c r="N5" s="37">
+        <v>0</v>
+      </c>
+      <c r="O5" s="37">
+        <v>0</v>
+      </c>
+      <c r="P5" s="37">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="37">
+        <v>0</v>
+      </c>
+      <c r="R5" s="37">
+        <v>0</v>
+      </c>
+      <c r="S5" s="37">
+        <v>0</v>
+      </c>
+      <c r="T5" s="37">
+        <v>0</v>
+      </c>
+      <c r="U5" s="37">
+        <v>0</v>
+      </c>
+      <c r="V5" s="37">
+        <v>0</v>
+      </c>
+      <c r="W5" s="37">
+        <v>0</v>
+      </c>
+      <c r="X5" s="37">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="37">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6" s="30">
+        <v>81</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="31">
+        <v>0</v>
+      </c>
+      <c r="D6" s="31">
+        <v>0</v>
+      </c>
+      <c r="E6" s="31">
+        <v>0</v>
+      </c>
+      <c r="F6" s="31">
+        <v>0</v>
+      </c>
+      <c r="G6" s="31">
+        <v>0</v>
+      </c>
+      <c r="H6" s="31">
+        <v>0</v>
+      </c>
+      <c r="I6" s="31">
+        <v>0</v>
+      </c>
+      <c r="J6" s="31">
+        <v>0</v>
+      </c>
+      <c r="K6" s="31">
+        <v>0</v>
+      </c>
+      <c r="L6" s="31">
+        <v>0</v>
+      </c>
+      <c r="M6" s="31">
+        <v>0</v>
+      </c>
+      <c r="N6" s="31">
+        <v>0</v>
+      </c>
+      <c r="O6" s="31">
+        <v>0</v>
+      </c>
+      <c r="P6" s="31">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="31">
+        <v>0</v>
+      </c>
+      <c r="R6" s="31">
+        <v>0</v>
+      </c>
+      <c r="S6" s="31">
+        <v>0</v>
+      </c>
+      <c r="T6" s="31">
+        <v>0</v>
+      </c>
+      <c r="U6" s="31">
+        <v>0</v>
+      </c>
+      <c r="V6" s="31">
+        <v>0</v>
+      </c>
+      <c r="W6" s="31">
+        <v>0</v>
+      </c>
+      <c r="X6" s="31">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="31">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" s="36">
+        <v>81</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="37">
+        <v>0</v>
+      </c>
+      <c r="D7" s="37">
+        <v>0</v>
+      </c>
+      <c r="E7" s="37">
+        <v>0</v>
+      </c>
+      <c r="F7" s="37">
+        <v>0</v>
+      </c>
+      <c r="G7" s="37">
+        <v>0</v>
+      </c>
+      <c r="H7" s="37">
+        <v>0</v>
+      </c>
+      <c r="I7" s="37">
+        <v>0</v>
+      </c>
+      <c r="J7" s="37">
+        <v>0</v>
+      </c>
+      <c r="K7" s="37">
+        <v>0</v>
+      </c>
+      <c r="L7" s="37">
+        <v>0</v>
+      </c>
+      <c r="M7" s="37">
+        <v>0</v>
+      </c>
+      <c r="N7" s="37">
+        <v>0</v>
+      </c>
+      <c r="O7" s="37">
+        <v>0</v>
+      </c>
+      <c r="P7" s="37">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="37">
+        <v>0</v>
+      </c>
+      <c r="R7" s="37">
+        <v>0</v>
+      </c>
+      <c r="S7" s="37">
+        <v>0</v>
+      </c>
+      <c r="T7" s="37">
+        <v>0</v>
+      </c>
+      <c r="U7" s="37">
+        <v>0</v>
+      </c>
+      <c r="V7" s="37">
+        <v>0</v>
+      </c>
+      <c r="W7" s="37">
+        <v>0</v>
+      </c>
+      <c r="X7" s="37">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="37">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" s="30">
+        <v>81</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="31">
+        <v>0</v>
+      </c>
+      <c r="D8" s="31">
+        <v>0</v>
+      </c>
+      <c r="E8" s="31">
+        <v>0</v>
+      </c>
+      <c r="F8" s="31">
+        <v>0</v>
+      </c>
+      <c r="G8" s="31">
+        <v>0</v>
+      </c>
+      <c r="H8" s="31">
+        <v>0</v>
+      </c>
+      <c r="I8" s="31">
+        <v>0</v>
+      </c>
+      <c r="J8" s="31">
+        <v>0</v>
+      </c>
+      <c r="K8" s="31">
+        <v>0</v>
+      </c>
+      <c r="L8" s="31">
+        <v>0</v>
+      </c>
+      <c r="M8" s="31">
+        <v>0</v>
+      </c>
+      <c r="N8" s="31">
+        <v>0</v>
+      </c>
+      <c r="O8" s="31">
+        <v>0</v>
+      </c>
+      <c r="P8" s="31">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="31">
+        <v>0</v>
+      </c>
+      <c r="R8" s="31">
+        <v>0</v>
+      </c>
+      <c r="S8" s="31">
+        <v>0</v>
+      </c>
+      <c r="T8" s="31">
+        <v>0</v>
+      </c>
+      <c r="U8" s="31">
+        <v>0</v>
+      </c>
+      <c r="V8" s="31">
+        <v>0</v>
+      </c>
+      <c r="W8" s="31">
+        <v>0</v>
+      </c>
+      <c r="X8" s="31">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="31">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="37">
+        <v>0</v>
+      </c>
+      <c r="D9" s="37">
+        <v>0</v>
+      </c>
+      <c r="E9" s="37">
+        <v>0</v>
+      </c>
+      <c r="F9" s="37">
+        <v>0</v>
+      </c>
+      <c r="G9" s="37">
+        <v>0</v>
+      </c>
+      <c r="H9" s="37">
+        <v>0</v>
+      </c>
+      <c r="I9" s="37">
+        <v>0</v>
+      </c>
+      <c r="J9" s="37">
+        <v>0</v>
+      </c>
+      <c r="K9" s="37">
+        <v>0</v>
+      </c>
+      <c r="L9" s="37">
+        <v>0</v>
+      </c>
+      <c r="M9" s="37">
+        <v>0</v>
+      </c>
+      <c r="N9" s="37">
+        <v>0</v>
+      </c>
+      <c r="O9" s="37">
+        <v>0</v>
+      </c>
+      <c r="P9" s="37">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="37">
+        <v>0</v>
+      </c>
+      <c r="R9" s="37">
+        <v>0</v>
+      </c>
+      <c r="S9" s="37">
+        <v>0</v>
+      </c>
+      <c r="T9" s="37">
+        <v>0</v>
+      </c>
+      <c r="U9" s="37">
+        <v>0</v>
+      </c>
+      <c r="V9" s="37">
+        <v>0</v>
+      </c>
+      <c r="W9" s="37">
+        <v>0</v>
+      </c>
+      <c r="X9" s="37">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="37">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="31">
+        <v>0</v>
+      </c>
+      <c r="D10" s="31">
+        <v>0</v>
+      </c>
+      <c r="E10" s="31">
+        <v>0</v>
+      </c>
+      <c r="F10" s="31">
+        <v>0</v>
+      </c>
+      <c r="G10" s="31">
+        <v>0</v>
+      </c>
+      <c r="H10" s="31">
+        <v>0</v>
+      </c>
+      <c r="I10" s="31">
+        <v>0</v>
+      </c>
+      <c r="J10" s="31">
+        <v>0</v>
+      </c>
+      <c r="K10" s="31">
+        <v>0</v>
+      </c>
+      <c r="L10" s="31">
+        <v>0</v>
+      </c>
+      <c r="M10" s="31">
+        <v>0</v>
+      </c>
+      <c r="N10" s="31">
+        <v>0</v>
+      </c>
+      <c r="O10" s="31">
+        <v>0</v>
+      </c>
+      <c r="P10" s="31">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="31">
+        <v>0</v>
+      </c>
+      <c r="R10" s="31">
+        <v>0</v>
+      </c>
+      <c r="S10" s="31">
+        <v>0</v>
+      </c>
+      <c r="T10" s="31">
+        <v>0</v>
+      </c>
+      <c r="U10" s="31">
+        <v>0</v>
+      </c>
+      <c r="V10" s="31">
+        <v>0</v>
+      </c>
+      <c r="W10" s="31">
+        <v>0</v>
+      </c>
+      <c r="X10" s="31">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="31">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11" s="36">
+        <v>84</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="37">
+        <v>0</v>
+      </c>
+      <c r="D11" s="37">
+        <v>0</v>
+      </c>
+      <c r="E11" s="37">
+        <v>0</v>
+      </c>
+      <c r="F11" s="37">
+        <v>0</v>
+      </c>
+      <c r="G11" s="37">
+        <v>0</v>
+      </c>
+      <c r="H11" s="37">
+        <v>0</v>
+      </c>
+      <c r="I11" s="37">
+        <v>0</v>
+      </c>
+      <c r="J11" s="37">
+        <v>0</v>
+      </c>
+      <c r="K11" s="37">
+        <v>0</v>
+      </c>
+      <c r="L11" s="37">
+        <v>0</v>
+      </c>
+      <c r="M11" s="37">
+        <v>0</v>
+      </c>
+      <c r="N11" s="37">
+        <v>0</v>
+      </c>
+      <c r="O11" s="37">
+        <v>0</v>
+      </c>
+      <c r="P11" s="37">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="37">
+        <v>0</v>
+      </c>
+      <c r="R11" s="37">
+        <v>0</v>
+      </c>
+      <c r="S11" s="37">
+        <v>0</v>
+      </c>
+      <c r="T11" s="37">
+        <v>0</v>
+      </c>
+      <c r="U11" s="37">
+        <v>0</v>
+      </c>
+      <c r="V11" s="37">
+        <v>0</v>
+      </c>
+      <c r="W11" s="37">
+        <v>0</v>
+      </c>
+      <c r="X11" s="37">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="37">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="31">
+        <v>0</v>
+      </c>
+      <c r="D12" s="31">
+        <v>0</v>
+      </c>
+      <c r="E12" s="31">
+        <v>0</v>
+      </c>
+      <c r="F12" s="31">
+        <v>0</v>
+      </c>
+      <c r="G12" s="31">
+        <v>0</v>
+      </c>
+      <c r="H12" s="31">
+        <v>0</v>
+      </c>
+      <c r="I12" s="31">
+        <v>0</v>
+      </c>
+      <c r="J12" s="31">
+        <v>0</v>
+      </c>
+      <c r="K12" s="31">
+        <v>0</v>
+      </c>
+      <c r="L12" s="31">
+        <v>0</v>
+      </c>
+      <c r="M12" s="31">
+        <v>0</v>
+      </c>
+      <c r="N12" s="31">
+        <v>0</v>
+      </c>
+      <c r="O12" s="31">
+        <v>0</v>
+      </c>
+      <c r="P12" s="31">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="31">
+        <v>0</v>
+      </c>
+      <c r="R12" s="31">
+        <v>0</v>
+      </c>
+      <c r="S12" s="31">
+        <v>0</v>
+      </c>
+      <c r="T12" s="31">
+        <v>0</v>
+      </c>
+      <c r="U12" s="31">
+        <v>0</v>
+      </c>
+      <c r="V12" s="31">
+        <v>0</v>
+      </c>
+      <c r="W12" s="31">
+        <v>0</v>
+      </c>
+      <c r="X12" s="31">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="31">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="37">
+        <v>0</v>
+      </c>
+      <c r="D13" s="37">
+        <v>0</v>
+      </c>
+      <c r="E13" s="37">
+        <v>0</v>
+      </c>
+      <c r="F13" s="37">
+        <v>0</v>
+      </c>
+      <c r="G13" s="37">
+        <v>0</v>
+      </c>
+      <c r="H13" s="37">
+        <v>0</v>
+      </c>
+      <c r="I13" s="37">
+        <v>0</v>
+      </c>
+      <c r="J13" s="37">
+        <v>0</v>
+      </c>
+      <c r="K13" s="37">
+        <v>0</v>
+      </c>
+      <c r="L13" s="37">
+        <v>0</v>
+      </c>
+      <c r="M13" s="37">
+        <v>0</v>
+      </c>
+      <c r="N13" s="37">
+        <v>0</v>
+      </c>
+      <c r="O13" s="37">
+        <v>0</v>
+      </c>
+      <c r="P13" s="37">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="37">
+        <v>0</v>
+      </c>
+      <c r="R13" s="37">
+        <v>0</v>
+      </c>
+      <c r="S13" s="37">
+        <v>0</v>
+      </c>
+      <c r="T13" s="37">
+        <v>0</v>
+      </c>
+      <c r="U13" s="37">
+        <v>0</v>
+      </c>
+      <c r="V13" s="37">
+        <v>0</v>
+      </c>
+      <c r="W13" s="37">
+        <v>0</v>
+      </c>
+      <c r="X13" s="37">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="37">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="34">
+        <v>0</v>
+      </c>
+      <c r="D14" s="34">
+        <v>0</v>
+      </c>
+      <c r="E14" s="34">
+        <v>0</v>
+      </c>
+      <c r="F14" s="34">
+        <v>0</v>
+      </c>
+      <c r="G14" s="34">
+        <v>0</v>
+      </c>
+      <c r="H14" s="34">
+        <v>0</v>
+      </c>
+      <c r="I14" s="34">
+        <v>0</v>
+      </c>
+      <c r="J14" s="34">
+        <v>0</v>
+      </c>
+      <c r="K14" s="34">
+        <v>0</v>
+      </c>
+      <c r="L14" s="34">
+        <v>0</v>
+      </c>
+      <c r="M14" s="34">
+        <v>0</v>
+      </c>
+      <c r="N14" s="34">
+        <v>0</v>
+      </c>
+      <c r="O14" s="34">
+        <v>0</v>
+      </c>
+      <c r="P14" s="34">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="34">
+        <v>0</v>
+      </c>
+      <c r="R14" s="34">
+        <v>0</v>
+      </c>
+      <c r="S14" s="34">
+        <v>0</v>
+      </c>
+      <c r="T14" s="34">
+        <v>0</v>
+      </c>
+      <c r="U14" s="34">
+        <v>0</v>
+      </c>
+      <c r="V14" s="34">
+        <v>0</v>
+      </c>
+      <c r="W14" s="34">
+        <v>0</v>
+      </c>
+      <c r="X14" s="34">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="34">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="35">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -771,12 +2089,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA9D8965-069B-4667-A351-BA2CC7871A2D}">
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="C1" sqref="C1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,16 +2129,16 @@
         <v>18</v>
       </c>
       <c r="I1" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="L1" s="27" t="s">
-        <v>22</v>
+        <v>41</v>
+      </c>
+      <c r="J1" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" s="39" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1095,164 +2413,1385 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B5E9472-F4F9-472D-A559-24D5CE8770E9}">
-  <dimension ref="A1:AA14"/>
+  <dimension ref="A1:AL15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
+    <sheetView topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" style="1" customWidth="1"/>
-    <col min="2" max="3" width="14.5703125" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="1"/>
+    <col min="5" max="38" width="17.7109375" style="1" customWidth="1"/>
+    <col min="39" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:38" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="F1" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="H1" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="N1" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="O1" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="P1" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="R1" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="30" t="s">
+      <c r="S1" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="T1" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="U1" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="V1" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="W1" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="X1" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y1" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z1" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA1" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB1" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC1" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD1" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE1" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF1" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG1" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="AH1" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="AI1" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ1" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="AK1" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL1" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A2" s="30">
+        <v>83</v>
+      </c>
+      <c r="B2" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="C2" s="31">
+        <v>-65</v>
+      </c>
+      <c r="D2" s="31">
+        <v>275</v>
+      </c>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31">
+        <v>20</v>
+      </c>
+      <c r="H2" s="31">
+        <v>2000</v>
+      </c>
+      <c r="I2" s="31">
+        <v>20</v>
+      </c>
+      <c r="J2" s="31">
+        <v>2000</v>
+      </c>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31">
+        <v>20</v>
+      </c>
+      <c r="N2" s="31">
+        <v>2000</v>
+      </c>
+      <c r="O2" s="31">
+        <v>20</v>
+      </c>
+      <c r="P2" s="31">
+        <v>2000</v>
+      </c>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31">
+        <v>20</v>
+      </c>
+      <c r="T2" s="31">
+        <v>2000</v>
+      </c>
+      <c r="U2" s="31">
+        <v>20</v>
+      </c>
+      <c r="V2" s="31">
+        <v>2000</v>
+      </c>
+      <c r="W2" s="31">
+        <v>20</v>
+      </c>
+      <c r="X2" s="31">
+        <v>2000</v>
+      </c>
+      <c r="Y2" s="31">
+        <v>20</v>
+      </c>
+      <c r="Z2" s="31">
+        <v>2000</v>
+      </c>
+      <c r="AA2" s="31">
+        <v>20</v>
+      </c>
+      <c r="AB2" s="31">
+        <v>2000</v>
+      </c>
+      <c r="AC2" s="31">
+        <v>20</v>
+      </c>
+      <c r="AD2" s="31">
+        <v>2000</v>
+      </c>
+      <c r="AE2" s="31">
+        <v>20</v>
+      </c>
+      <c r="AF2" s="31">
+        <v>2000</v>
+      </c>
+      <c r="AG2" s="31">
+        <v>20</v>
+      </c>
+      <c r="AH2" s="31">
+        <v>2000</v>
+      </c>
+      <c r="AI2" s="31">
+        <v>20</v>
+      </c>
+      <c r="AJ2" s="31">
+        <v>1620</v>
+      </c>
+      <c r="AK2" s="31">
+        <v>20</v>
+      </c>
+      <c r="AL2" s="32">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A3" s="36">
+        <v>83</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="37">
+        <v>-15</v>
+      </c>
+      <c r="D3" s="37">
+        <v>400</v>
+      </c>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37">
+        <v>20</v>
+      </c>
+      <c r="H3" s="37">
+        <v>2000</v>
+      </c>
+      <c r="I3" s="37">
+        <v>20</v>
+      </c>
+      <c r="J3" s="37">
+        <v>2000</v>
+      </c>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="37">
+        <v>20</v>
+      </c>
+      <c r="N3" s="37">
+        <v>2000</v>
+      </c>
+      <c r="O3" s="37">
+        <v>20</v>
+      </c>
+      <c r="P3" s="37">
+        <v>2000</v>
+      </c>
+      <c r="Q3" s="37"/>
+      <c r="R3" s="37"/>
+      <c r="S3" s="37">
+        <v>20</v>
+      </c>
+      <c r="T3" s="37">
+        <v>2000</v>
+      </c>
+      <c r="U3" s="37">
+        <v>20</v>
+      </c>
+      <c r="V3" s="37">
+        <v>2000</v>
+      </c>
+      <c r="W3" s="37">
+        <v>20</v>
+      </c>
+      <c r="X3" s="37">
+        <v>2000</v>
+      </c>
+      <c r="Y3" s="37">
+        <v>20</v>
+      </c>
+      <c r="Z3" s="37">
+        <v>2000</v>
+      </c>
+      <c r="AA3" s="37">
+        <v>20</v>
+      </c>
+      <c r="AB3" s="37">
+        <v>2000</v>
+      </c>
+      <c r="AC3" s="37">
+        <v>20</v>
+      </c>
+      <c r="AD3" s="37">
+        <v>2000</v>
+      </c>
+      <c r="AE3" s="37">
+        <v>20</v>
+      </c>
+      <c r="AF3" s="37">
+        <v>2000</v>
+      </c>
+      <c r="AG3" s="37">
+        <v>20</v>
+      </c>
+      <c r="AH3" s="37">
+        <v>2000</v>
+      </c>
+      <c r="AI3" s="37">
+        <v>20</v>
+      </c>
+      <c r="AJ3" s="37">
+        <v>1620</v>
+      </c>
+      <c r="AK3" s="37">
+        <v>20</v>
+      </c>
+      <c r="AL3" s="38">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A4" s="30">
+        <v>83</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="31">
+        <v>-65</v>
+      </c>
+      <c r="D4" s="31">
+        <v>300</v>
+      </c>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31">
+        <v>20</v>
+      </c>
+      <c r="H4" s="31">
+        <v>2000</v>
+      </c>
+      <c r="I4" s="31">
+        <v>20</v>
+      </c>
+      <c r="J4" s="31">
+        <v>2000</v>
+      </c>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31">
+        <v>20</v>
+      </c>
+      <c r="N4" s="31">
+        <v>2000</v>
+      </c>
+      <c r="O4" s="31">
+        <v>20</v>
+      </c>
+      <c r="P4" s="31">
+        <v>2000</v>
+      </c>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="31"/>
+      <c r="S4" s="31">
+        <v>20</v>
+      </c>
+      <c r="T4" s="31">
+        <v>2000</v>
+      </c>
+      <c r="U4" s="31">
+        <v>20</v>
+      </c>
+      <c r="V4" s="31">
+        <v>2000</v>
+      </c>
+      <c r="W4" s="31">
+        <v>20</v>
+      </c>
+      <c r="X4" s="31">
+        <v>2000</v>
+      </c>
+      <c r="Y4" s="31">
+        <v>20</v>
+      </c>
+      <c r="Z4" s="31">
+        <v>2000</v>
+      </c>
+      <c r="AA4" s="31">
+        <v>20</v>
+      </c>
+      <c r="AB4" s="31">
+        <v>2000</v>
+      </c>
+      <c r="AC4" s="31">
+        <v>20</v>
+      </c>
+      <c r="AD4" s="31">
+        <v>2000</v>
+      </c>
+      <c r="AE4" s="31">
+        <v>20</v>
+      </c>
+      <c r="AF4" s="31">
+        <v>2000</v>
+      </c>
+      <c r="AG4" s="31">
+        <v>20</v>
+      </c>
+      <c r="AH4" s="31">
+        <v>2000</v>
+      </c>
+      <c r="AI4" s="31">
+        <v>20</v>
+      </c>
+      <c r="AJ4" s="31">
+        <v>1620</v>
+      </c>
+      <c r="AK4" s="31">
+        <v>20</v>
+      </c>
+      <c r="AL4" s="32">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A5" s="36">
+        <v>83</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="37">
+        <v>0</v>
+      </c>
+      <c r="D5" s="37">
+        <v>550</v>
+      </c>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37">
+        <v>20</v>
+      </c>
+      <c r="H5" s="37">
+        <v>2000</v>
+      </c>
+      <c r="I5" s="37">
+        <v>20</v>
+      </c>
+      <c r="J5" s="37">
+        <v>2000</v>
+      </c>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="37">
+        <v>20</v>
+      </c>
+      <c r="N5" s="37">
+        <v>2000</v>
+      </c>
+      <c r="O5" s="37">
+        <v>20</v>
+      </c>
+      <c r="P5" s="37">
+        <v>2000</v>
+      </c>
+      <c r="Q5" s="37"/>
+      <c r="R5" s="37"/>
+      <c r="S5" s="37">
+        <v>20</v>
+      </c>
+      <c r="T5" s="37">
+        <v>2000</v>
+      </c>
+      <c r="U5" s="37">
+        <v>20</v>
+      </c>
+      <c r="V5" s="37">
+        <v>2000</v>
+      </c>
+      <c r="W5" s="37">
+        <v>20</v>
+      </c>
+      <c r="X5" s="37">
+        <v>2000</v>
+      </c>
+      <c r="Y5" s="37">
+        <v>20</v>
+      </c>
+      <c r="Z5" s="37">
+        <v>2000</v>
+      </c>
+      <c r="AA5" s="37">
+        <v>20</v>
+      </c>
+      <c r="AB5" s="37">
+        <v>2000</v>
+      </c>
+      <c r="AC5" s="37">
+        <v>20</v>
+      </c>
+      <c r="AD5" s="37">
+        <v>2000</v>
+      </c>
+      <c r="AE5" s="37">
+        <v>20</v>
+      </c>
+      <c r="AF5" s="37">
+        <v>2000</v>
+      </c>
+      <c r="AG5" s="37">
+        <v>20</v>
+      </c>
+      <c r="AH5" s="37">
+        <v>2000</v>
+      </c>
+      <c r="AI5" s="37">
+        <v>20</v>
+      </c>
+      <c r="AJ5" s="37">
+        <v>1620</v>
+      </c>
+      <c r="AK5" s="37">
+        <v>20</v>
+      </c>
+      <c r="AL5" s="38">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A6" s="30">
+        <v>81</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="31">
+        <v>-423</v>
+      </c>
+      <c r="D6" s="31">
+        <v>400</v>
+      </c>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31">
+        <v>50</v>
+      </c>
+      <c r="H6" s="31">
+        <v>1000</v>
+      </c>
+      <c r="I6" s="31">
+        <v>50</v>
+      </c>
+      <c r="J6" s="31">
+        <v>1000</v>
+      </c>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31">
+        <v>50</v>
+      </c>
+      <c r="N6" s="31">
+        <v>900</v>
+      </c>
+      <c r="O6" s="31">
+        <v>50</v>
+      </c>
+      <c r="P6" s="31">
+        <v>900</v>
+      </c>
+      <c r="Q6" s="31"/>
+      <c r="R6" s="31"/>
+      <c r="S6" s="31">
+        <v>50</v>
+      </c>
+      <c r="T6" s="31">
+        <v>900</v>
+      </c>
+      <c r="U6" s="31">
+        <v>50</v>
+      </c>
+      <c r="V6" s="31">
+        <v>900</v>
+      </c>
+      <c r="W6" s="31">
+        <v>50</v>
+      </c>
+      <c r="X6" s="31">
+        <v>500</v>
+      </c>
+      <c r="Y6" s="31">
+        <v>50</v>
+      </c>
+      <c r="Z6" s="31">
+        <v>500</v>
+      </c>
+      <c r="AA6" s="31">
+        <v>50</v>
+      </c>
+      <c r="AB6" s="31">
+        <v>500</v>
+      </c>
+      <c r="AC6" s="31">
+        <v>50</v>
+      </c>
+      <c r="AD6" s="31">
+        <v>500</v>
+      </c>
+      <c r="AE6" s="31">
+        <v>50</v>
+      </c>
+      <c r="AF6" s="31">
+        <v>500</v>
+      </c>
+      <c r="AG6" s="31">
+        <v>50</v>
+      </c>
+      <c r="AH6" s="31">
+        <v>500</v>
+      </c>
+      <c r="AI6" s="31">
+        <v>50</v>
+      </c>
+      <c r="AJ6" s="31">
+        <v>500</v>
+      </c>
+      <c r="AK6" s="31">
+        <v>50</v>
+      </c>
+      <c r="AL6" s="32">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A7" s="36">
+        <v>81</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="37">
+        <v>-423</v>
+      </c>
+      <c r="D7" s="37">
+        <v>300</v>
+      </c>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37">
+        <v>1001</v>
+      </c>
+      <c r="H7" s="37">
+        <v>4000</v>
+      </c>
+      <c r="I7" s="37">
+        <v>1001</v>
+      </c>
+      <c r="J7" s="37">
+        <v>4000</v>
+      </c>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="37">
+        <v>901</v>
+      </c>
+      <c r="N7" s="37">
+        <v>1500</v>
+      </c>
+      <c r="O7" s="37">
+        <v>901</v>
+      </c>
+      <c r="P7" s="37">
+        <v>1500</v>
+      </c>
+      <c r="Q7" s="37"/>
+      <c r="R7" s="37"/>
+      <c r="S7" s="37">
+        <v>901</v>
+      </c>
+      <c r="T7" s="37">
+        <v>1500</v>
+      </c>
+      <c r="U7" s="37">
+        <v>901</v>
+      </c>
+      <c r="V7" s="37">
+        <v>1500</v>
+      </c>
+      <c r="W7" s="37">
+        <v>501</v>
+      </c>
+      <c r="X7" s="37">
+        <v>750</v>
+      </c>
+      <c r="Y7" s="37">
+        <v>501</v>
+      </c>
+      <c r="Z7" s="37">
+        <v>750</v>
+      </c>
+      <c r="AA7" s="37">
+        <v>501</v>
+      </c>
+      <c r="AB7" s="37">
+        <v>750</v>
+      </c>
+      <c r="AC7" s="37">
+        <v>501</v>
+      </c>
+      <c r="AD7" s="37">
+        <v>750</v>
+      </c>
+      <c r="AE7" s="37">
+        <v>501</v>
+      </c>
+      <c r="AF7" s="37">
+        <v>750</v>
+      </c>
+      <c r="AG7" s="37">
+        <v>501</v>
+      </c>
+      <c r="AH7" s="37">
+        <v>750</v>
+      </c>
+      <c r="AI7" s="37">
+        <v>501</v>
+      </c>
+      <c r="AJ7" s="37">
+        <v>750</v>
+      </c>
+      <c r="AK7" s="37">
+        <v>501</v>
+      </c>
+      <c r="AL7" s="38">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A8" s="30">
+        <v>81</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="31">
+        <v>-423</v>
+      </c>
+      <c r="D8" s="31">
+        <v>500</v>
+      </c>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31">
+        <v>4001</v>
+      </c>
+      <c r="J8" s="31">
+        <v>10000</v>
+      </c>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31">
+        <v>1501</v>
+      </c>
+      <c r="N8" s="31">
+        <v>9600</v>
+      </c>
+      <c r="O8" s="31">
+        <v>1501</v>
+      </c>
+      <c r="P8" s="31">
+        <v>9600</v>
+      </c>
+      <c r="Q8" s="31"/>
+      <c r="R8" s="31"/>
+      <c r="S8" s="31">
+        <v>1501</v>
+      </c>
+      <c r="T8" s="31">
+        <v>4000</v>
+      </c>
+      <c r="U8" s="31">
+        <v>1501</v>
+      </c>
+      <c r="V8" s="31">
+        <v>4000</v>
+      </c>
+      <c r="W8" s="31">
+        <v>751</v>
+      </c>
+      <c r="X8" s="31">
+        <v>2990</v>
+      </c>
+      <c r="Y8" s="31">
+        <v>751</v>
+      </c>
+      <c r="Z8" s="31">
+        <v>4040</v>
+      </c>
+      <c r="AA8" s="31">
+        <v>752</v>
+      </c>
+      <c r="AB8" s="31">
+        <v>2750</v>
+      </c>
+      <c r="AC8" s="31">
+        <v>751</v>
+      </c>
+      <c r="AD8" s="31">
+        <v>2570</v>
+      </c>
+      <c r="AE8" s="31">
+        <v>751</v>
+      </c>
+      <c r="AF8" s="31">
+        <v>2270</v>
+      </c>
+      <c r="AG8" s="31">
+        <v>751</v>
+      </c>
+      <c r="AH8" s="31">
+        <v>2580</v>
+      </c>
+      <c r="AI8" s="31">
+        <v>751</v>
+      </c>
+      <c r="AJ8" s="31">
+        <v>1620</v>
+      </c>
+      <c r="AK8" s="31">
+        <v>751</v>
+      </c>
+      <c r="AL8" s="32">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A9" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="37">
+        <v>-65</v>
+      </c>
+      <c r="D9" s="37">
+        <v>400</v>
+      </c>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37">
+        <v>50</v>
+      </c>
+      <c r="H9" s="37">
+        <v>2000</v>
+      </c>
+      <c r="I9" s="37">
+        <v>50</v>
+      </c>
+      <c r="J9" s="37">
+        <v>2000</v>
+      </c>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37"/>
+      <c r="O9" s="37"/>
+      <c r="P9" s="37"/>
+      <c r="Q9" s="37"/>
+      <c r="R9" s="37"/>
+      <c r="S9" s="37">
+        <v>50</v>
+      </c>
+      <c r="T9" s="37">
+        <v>2000</v>
+      </c>
+      <c r="U9" s="37">
+        <v>50</v>
+      </c>
+      <c r="V9" s="37">
+        <v>2000</v>
+      </c>
+      <c r="W9" s="37"/>
+      <c r="X9" s="37"/>
+      <c r="Y9" s="37"/>
+      <c r="Z9" s="37"/>
+      <c r="AA9" s="37">
+        <v>50</v>
+      </c>
+      <c r="AB9" s="37">
+        <v>1000</v>
+      </c>
+      <c r="AC9" s="37">
+        <v>50</v>
+      </c>
+      <c r="AD9" s="37">
+        <v>1000</v>
+      </c>
+      <c r="AE9" s="37"/>
+      <c r="AF9" s="37"/>
+      <c r="AG9" s="37"/>
+      <c r="AH9" s="37"/>
+      <c r="AI9" s="37">
+        <v>50</v>
+      </c>
+      <c r="AJ9" s="37">
+        <v>1000</v>
+      </c>
+      <c r="AK9" s="37">
+        <v>50</v>
+      </c>
+      <c r="AL9" s="38">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A10" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="31">
+        <v>-65</v>
+      </c>
+      <c r="D10" s="31">
+        <v>300</v>
+      </c>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31">
+        <v>2001</v>
+      </c>
+      <c r="H10" s="31">
+        <v>4000</v>
+      </c>
+      <c r="I10" s="31">
+        <v>2001</v>
+      </c>
+      <c r="J10" s="31">
+        <v>6000</v>
+      </c>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="31"/>
+      <c r="O10" s="31"/>
+      <c r="P10" s="31"/>
+      <c r="Q10" s="31"/>
+      <c r="R10" s="31"/>
+      <c r="S10" s="31">
+        <v>2001</v>
+      </c>
+      <c r="T10" s="31">
+        <v>4000</v>
+      </c>
+      <c r="U10" s="31">
+        <v>2001</v>
+      </c>
+      <c r="V10" s="31">
+        <v>4000</v>
+      </c>
+      <c r="W10" s="31"/>
+      <c r="X10" s="31"/>
+      <c r="Y10" s="31"/>
+      <c r="Z10" s="31"/>
+      <c r="AA10" s="31">
+        <v>1001</v>
+      </c>
+      <c r="AB10" s="31">
+        <v>2570</v>
+      </c>
+      <c r="AC10" s="31">
+        <v>1001</v>
+      </c>
+      <c r="AD10" s="31">
+        <v>6000</v>
+      </c>
+      <c r="AE10" s="31"/>
+      <c r="AF10" s="31"/>
+      <c r="AG10" s="31"/>
+      <c r="AH10" s="31"/>
+      <c r="AI10" s="31">
+        <v>1001</v>
+      </c>
+      <c r="AJ10" s="31">
+        <v>1620</v>
+      </c>
+      <c r="AK10" s="31">
+        <v>1001</v>
+      </c>
+      <c r="AL10" s="32">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A11" s="36">
+        <v>84</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="37">
+        <v>-40</v>
+      </c>
+      <c r="D11" s="37">
+        <v>300</v>
+      </c>
+      <c r="E11" s="37">
+        <v>6000</v>
+      </c>
+      <c r="F11" s="37">
+        <v>21756</v>
+      </c>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="37"/>
+      <c r="L11" s="37"/>
+      <c r="M11" s="37"/>
+      <c r="N11" s="37"/>
+      <c r="O11" s="37"/>
+      <c r="P11" s="37"/>
+      <c r="Q11" s="37"/>
+      <c r="R11" s="37"/>
+      <c r="S11" s="37"/>
+      <c r="T11" s="37"/>
+      <c r="U11" s="37"/>
+      <c r="V11" s="37"/>
+      <c r="W11" s="37"/>
+      <c r="X11" s="37"/>
+      <c r="Y11" s="37"/>
+      <c r="Z11" s="37"/>
+      <c r="AA11" s="37"/>
+      <c r="AB11" s="37"/>
+      <c r="AC11" s="37"/>
+      <c r="AD11" s="37"/>
+      <c r="AE11" s="37"/>
+      <c r="AF11" s="37"/>
+      <c r="AG11" s="37"/>
+      <c r="AH11" s="37"/>
+      <c r="AI11" s="37"/>
+      <c r="AJ11" s="37"/>
+      <c r="AK11" s="37"/>
+      <c r="AL11" s="38"/>
+    </row>
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A12" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="31">
+        <v>-65</v>
+      </c>
+      <c r="D12" s="31">
+        <v>275</v>
+      </c>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31">
+        <v>37</v>
+      </c>
+      <c r="L12" s="31">
+        <v>531</v>
+      </c>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="31"/>
+      <c r="P12" s="31"/>
+      <c r="Q12" s="31">
+        <v>45</v>
+      </c>
+      <c r="R12" s="31">
+        <v>374</v>
+      </c>
+      <c r="S12" s="31"/>
+      <c r="T12" s="31"/>
+      <c r="U12" s="31"/>
+      <c r="V12" s="31"/>
+      <c r="W12" s="31"/>
+      <c r="X12" s="31"/>
+      <c r="Y12" s="31"/>
+      <c r="Z12" s="31"/>
+      <c r="AA12" s="31"/>
+      <c r="AB12" s="31"/>
+      <c r="AC12" s="31"/>
+      <c r="AD12" s="31"/>
+      <c r="AE12" s="31"/>
+      <c r="AF12" s="31"/>
+      <c r="AG12" s="31"/>
+      <c r="AH12" s="31"/>
+      <c r="AI12" s="31"/>
+      <c r="AJ12" s="31"/>
+      <c r="AK12" s="31"/>
+      <c r="AL12" s="32"/>
+    </row>
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A13" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="37">
+        <v>-15</v>
+      </c>
+      <c r="D13" s="37">
+        <v>400</v>
+      </c>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="37">
+        <v>37</v>
+      </c>
+      <c r="L13" s="37">
+        <v>531</v>
+      </c>
+      <c r="M13" s="37"/>
+      <c r="N13" s="37"/>
+      <c r="O13" s="37"/>
+      <c r="P13" s="37"/>
+      <c r="Q13" s="37">
+        <v>45</v>
+      </c>
+      <c r="R13" s="37">
+        <v>374</v>
+      </c>
+      <c r="S13" s="37"/>
+      <c r="T13" s="37"/>
+      <c r="U13" s="37"/>
+      <c r="V13" s="37"/>
+      <c r="W13" s="37"/>
+      <c r="X13" s="37"/>
+      <c r="Y13" s="37"/>
+      <c r="Z13" s="37"/>
+      <c r="AA13" s="37"/>
+      <c r="AB13" s="37"/>
+      <c r="AC13" s="37"/>
+      <c r="AD13" s="37"/>
+      <c r="AE13" s="37"/>
+      <c r="AF13" s="37"/>
+      <c r="AG13" s="37"/>
+      <c r="AH13" s="37"/>
+      <c r="AI13" s="37"/>
+      <c r="AJ13" s="37"/>
+      <c r="AK13" s="37"/>
+      <c r="AL13" s="38"/>
+    </row>
+    <row r="14" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="34">
+        <v>-65</v>
+      </c>
+      <c r="D14" s="34">
+        <v>300</v>
+      </c>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34">
+        <v>371</v>
+      </c>
+      <c r="L14" s="34">
+        <v>531</v>
+      </c>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="34"/>
+      <c r="P14" s="34"/>
+      <c r="Q14" s="34">
+        <v>45</v>
+      </c>
+      <c r="R14" s="34">
+        <v>374</v>
+      </c>
+      <c r="S14" s="34"/>
+      <c r="T14" s="34"/>
+      <c r="U14" s="34"/>
+      <c r="V14" s="34"/>
+      <c r="W14" s="34"/>
+      <c r="X14" s="34"/>
+      <c r="Y14" s="34"/>
+      <c r="Z14" s="34"/>
+      <c r="AA14" s="34"/>
+      <c r="AB14" s="34"/>
+      <c r="AC14" s="34"/>
+      <c r="AD14" s="34"/>
+      <c r="AE14" s="34"/>
+      <c r="AF14" s="34"/>
+      <c r="AG14" s="34"/>
+      <c r="AH14" s="34"/>
+      <c r="AI14" s="34"/>
+      <c r="AJ14" s="34"/>
+      <c r="AK14" s="34"/>
+      <c r="AL14" s="35"/>
+    </row>
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="I15" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54E22345-509C-416A-AFD4-EF21375FF1C4}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="30" t="s">
+      <c r="B1" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="31">
+        <v>-325</v>
+      </c>
+      <c r="C2" s="32">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="37">
+        <v>-20</v>
+      </c>
+      <c r="C3" s="38">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" s="30" t="s">
+      <c r="B4" s="34">
+        <v>-423</v>
+      </c>
+      <c r="C4" s="35">
+        <v>550</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D368A94-4BF2-45ED-863C-19D230F439F9}">
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="M1" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="N1" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="O1" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="P1" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q1" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="R1" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="S1" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="T1" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="U1" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="V1" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="W1" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="X1" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y1" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z1" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA1" s="29" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>83</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="1">
-        <v>-65</v>
-      </c>
-      <c r="E2" s="1">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="J14" s="1" t="s">
-        <v>49</v>
+      <c r="B4" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
significant progress on relief valve selector function
</commit_message>
<xml_diff>
--- a/Relief Valve Selector/ReliefValveSelectorReference.xlsx
+++ b/Relief Valve Selector/ReliefValveSelectorReference.xlsx
@@ -5,20 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AustinThomas\Desktop\MATLAB\MARS\Relief Valve Selector\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AustinThomas\Desktop\MDRT\Relief Valve Selector\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDEA375B-839A-47CD-A1D4-50A7EB4385B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB7C8F28-B9EC-4196-8910-210491A5AA42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32730" yWindow="1980" windowWidth="23010" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="7" r:id="rId1"/>
     <sheet name="CommodityRef" sheetId="1" r:id="rId2"/>
     <sheet name="ModelTypeRef" sheetId="3" r:id="rId3"/>
-    <sheet name="ThermoSeatRef" sheetId="4" r:id="rId4"/>
+    <sheet name="ThermoRef" sheetId="4" r:id="rId4"/>
     <sheet name="TempMaterialRef" sheetId="5" r:id="rId5"/>
-    <sheet name="SeatAndMatRef" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="108">
   <si>
     <t>Commodity</t>
   </si>
@@ -107,9 +106,6 @@
     <t>-7 P Max</t>
   </si>
   <si>
-    <t>Seat Material</t>
-  </si>
-  <si>
     <t>NBR</t>
   </si>
   <si>
@@ -119,9 +115,6 @@
     <t>SS</t>
   </si>
   <si>
-    <t xml:space="preserve">      </t>
-  </si>
-  <si>
     <t>FKM</t>
   </si>
   <si>
@@ -140,9 +133,6 @@
     <t>Vespel</t>
   </si>
   <si>
-    <t>CS</t>
-  </si>
-  <si>
     <t>Brass</t>
   </si>
   <si>
@@ -152,9 +142,6 @@
     <t>Arlon 300 XT</t>
   </si>
   <si>
-    <t>Type</t>
-  </si>
-  <si>
     <t>-F</t>
   </si>
   <si>
@@ -179,39 +166,18 @@
     <t>-4 P Max (Brass)</t>
   </si>
   <si>
-    <t>-4 P Min (CS/SS)</t>
-  </si>
-  <si>
-    <t>-4 P Max (CS/SS)</t>
-  </si>
-  <si>
     <t>-6 P Min (Brass)</t>
   </si>
   <si>
     <t>-6 P Max (Brass)</t>
   </si>
   <si>
-    <t>-6 P Min (CS/SS)</t>
-  </si>
-  <si>
-    <t>-6 P Max (CS/SS)</t>
-  </si>
-  <si>
     <t>-8 P Min (Brass)</t>
   </si>
   <si>
     <t>-8 P Max (Brass)</t>
   </si>
   <si>
-    <t>-F P Min (CS/SS)</t>
-  </si>
-  <si>
-    <t>-8 P Min (CS/SS)</t>
-  </si>
-  <si>
-    <t>-8 P Max (CS/SS)</t>
-  </si>
-  <si>
     <t>-F P Min (Brass)</t>
   </si>
   <si>
@@ -236,27 +202,6 @@
     <t>- J P Max (Brass)</t>
   </si>
   <si>
-    <t>-F P Max (CS/SS)</t>
-  </si>
-  <si>
-    <t>-G P Min (CS/SS)</t>
-  </si>
-  <si>
-    <t>-G P Max (CS/SS)</t>
-  </si>
-  <si>
-    <t>-H P Min (CS/SS)</t>
-  </si>
-  <si>
-    <t>-H P Max (CS/SS)</t>
-  </si>
-  <si>
-    <t>-J P Min (CS/SS)</t>
-  </si>
-  <si>
-    <t>- J P Max (CS/SS)</t>
-  </si>
-  <si>
     <t>-2 (SS)</t>
   </si>
   <si>
@@ -321,6 +266,93 @@
   </si>
   <si>
     <t>-J (SS)</t>
+  </si>
+  <si>
+    <t>-4 P Min (CS)</t>
+  </si>
+  <si>
+    <t>-4 P Max (CS)</t>
+  </si>
+  <si>
+    <t>-4 P Min (SS)</t>
+  </si>
+  <si>
+    <t>-4 P Max (SS)</t>
+  </si>
+  <si>
+    <t>-6 P Min (CS)</t>
+  </si>
+  <si>
+    <t>-6 P Max (CS)</t>
+  </si>
+  <si>
+    <t>-6 P Min (SS)</t>
+  </si>
+  <si>
+    <t>-6 P Max (SS)</t>
+  </si>
+  <si>
+    <t>-8 P Min (CS)</t>
+  </si>
+  <si>
+    <t>-8 P Max (CS)</t>
+  </si>
+  <si>
+    <t>-8 P Min (SS)</t>
+  </si>
+  <si>
+    <t>-8 P Max (SS)</t>
+  </si>
+  <si>
+    <t>-F P Min (CSC)</t>
+  </si>
+  <si>
+    <t>-F P Max (CS)</t>
+  </si>
+  <si>
+    <t>-F P Min (SS)</t>
+  </si>
+  <si>
+    <t>-F P Max (SS)</t>
+  </si>
+  <si>
+    <t>-G P Min (CS)</t>
+  </si>
+  <si>
+    <t>-G P Max (CS)</t>
+  </si>
+  <si>
+    <t>-G P Min (SS)</t>
+  </si>
+  <si>
+    <t>-G P Max (SS)</t>
+  </si>
+  <si>
+    <t>-H P Min (CS)</t>
+  </si>
+  <si>
+    <t>-H P Max (CS)</t>
+  </si>
+  <si>
+    <t>-H P Min (SS)</t>
+  </si>
+  <si>
+    <t>-H P Max (SS)</t>
+  </si>
+  <si>
+    <t>-J P Min (CS)</t>
+  </si>
+  <si>
+    <t>- J P Max (CS)</t>
+  </si>
+  <si>
+    <t>-J P Min (SS)</t>
+  </si>
+  <si>
+    <t>- J P Max (SS)</t>
+  </si>
+  <si>
+    <t>SeatMaterial</t>
   </si>
 </sst>
 </file>
@@ -471,7 +503,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -594,6 +626,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -879,7 +917,7 @@
   <dimension ref="A1:Z14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X25" sqref="X25"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,79 +933,79 @@
         <v>11</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>25</v>
+        <v>107</v>
       </c>
       <c r="C1" s="40" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="D1" s="40" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="E1" s="40" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="F1" s="40" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="G1" s="40" t="s">
         <v>15</v>
       </c>
       <c r="H1" s="40" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="I1" s="40" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="J1" s="40" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="K1" s="40" t="s">
         <v>17</v>
       </c>
       <c r="L1" s="40" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="M1" s="40" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="N1" s="40" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="O1" s="40" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="P1" s="40" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="Q1" s="40" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="R1" s="40" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="S1" s="40" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="T1" s="40" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="U1" s="40" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="V1" s="40" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="W1" s="40" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="X1" s="40" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="Y1" s="40" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="Z1" s="41" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
@@ -975,7 +1013,7 @@
         <v>83</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" s="31">
         <v>0</v>
@@ -1055,7 +1093,7 @@
         <v>83</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C3" s="37">
         <v>0</v>
@@ -1135,7 +1173,7 @@
         <v>83</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C4" s="31">
         <v>0</v>
@@ -1215,7 +1253,7 @@
         <v>83</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C5" s="37">
         <v>0</v>
@@ -1295,7 +1333,7 @@
         <v>81</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C6" s="31">
         <v>0</v>
@@ -1375,7 +1413,7 @@
         <v>81</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C7" s="37">
         <v>0</v>
@@ -1455,7 +1493,7 @@
         <v>81</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C8" s="31">
         <v>0</v>
@@ -1535,7 +1573,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C9" s="37">
         <v>0</v>
@@ -1615,7 +1653,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C10" s="31">
         <v>0</v>
@@ -1695,7 +1733,7 @@
         <v>84</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C11" s="37">
         <v>0</v>
@@ -1775,7 +1813,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="31">
         <v>0</v>
@@ -1855,7 +1893,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C13" s="37">
         <v>0</v>
@@ -1935,7 +1973,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C14" s="34">
         <v>0</v>
@@ -2094,7 +2132,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:L1"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2129,16 +2167,16 @@
         <v>18</v>
       </c>
       <c r="I1" s="28" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="J1" s="28" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="K1" s="28" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="L1" s="39" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -2415,10 +2453,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B5E9472-F4F9-472D-A559-24D5CE8770E9}">
-  <dimension ref="A1:AL15"/>
+  <dimension ref="A1:AZ14"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2426,132 +2464,174 @@
     <col min="1" max="1" width="13.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" style="1" customWidth="1"/>
     <col min="3" max="4" width="9.140625" style="1"/>
-    <col min="5" max="38" width="17.7109375" style="1" customWidth="1"/>
-    <col min="39" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="52" width="17.7109375" style="1" customWidth="1"/>
+    <col min="53" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:52" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="K1" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="L1" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="M1" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="P1" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q1" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="R1" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="S1" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="T1" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="U1" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="V1" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="W1" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="X1" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y1" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA1" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="AB1" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC1" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD1" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE1" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF1" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="AG1" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="AH1" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="AI1" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ1" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK1" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="AL1" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="AM1" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="AN1" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="AO1" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP1" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ1" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="AR1" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="AS1" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="AT1" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="AU1" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="AV1" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="AW1" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="AX1" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="AY1" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="AZ1" s="27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>83</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>25</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="I1" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="J1" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="K1" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="M1" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="N1" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="O1" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="P1" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q1" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="R1" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="S1" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="T1" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="U1" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="V1" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="W1" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="X1" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y1" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z1" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA1" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB1" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="AC1" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="AD1" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="AE1" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF1" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="AG1" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="AH1" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="AI1" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="AJ1" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="AK1" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="AL1" s="27" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A2" s="30">
-        <v>83</v>
-      </c>
-      <c r="B2" s="31" t="s">
-        <v>26</v>
       </c>
       <c r="C2" s="31">
         <v>-65</v>
@@ -2573,34 +2653,34 @@
       <c r="J2" s="31">
         <v>2000</v>
       </c>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31">
-        <v>20</v>
-      </c>
-      <c r="N2" s="31">
-        <v>2000</v>
-      </c>
+      <c r="K2" s="31">
+        <v>20</v>
+      </c>
+      <c r="L2" s="31">
+        <v>2000</v>
+      </c>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
       <c r="O2" s="31">
         <v>20</v>
       </c>
       <c r="P2" s="31">
         <v>2000</v>
       </c>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
+      <c r="Q2" s="31">
+        <v>20</v>
+      </c>
+      <c r="R2" s="31">
+        <v>2000</v>
+      </c>
       <c r="S2" s="31">
         <v>20</v>
       </c>
       <c r="T2" s="31">
         <v>2000</v>
       </c>
-      <c r="U2" s="31">
-        <v>20</v>
-      </c>
-      <c r="V2" s="31">
-        <v>2000</v>
-      </c>
+      <c r="U2" s="31"/>
+      <c r="V2" s="31"/>
       <c r="W2" s="31">
         <v>20</v>
       </c>
@@ -2641,21 +2721,63 @@
         <v>20</v>
       </c>
       <c r="AJ2" s="31">
+        <v>2000</v>
+      </c>
+      <c r="AK2" s="31">
+        <v>20</v>
+      </c>
+      <c r="AL2" s="31">
+        <v>2000</v>
+      </c>
+      <c r="AM2" s="31">
+        <v>20</v>
+      </c>
+      <c r="AN2" s="31">
+        <v>2000</v>
+      </c>
+      <c r="AO2" s="31">
+        <v>20</v>
+      </c>
+      <c r="AP2" s="31">
+        <v>2000</v>
+      </c>
+      <c r="AQ2" s="31">
+        <v>20</v>
+      </c>
+      <c r="AR2" s="31">
+        <v>2000</v>
+      </c>
+      <c r="AS2" s="31">
+        <v>20</v>
+      </c>
+      <c r="AT2" s="31">
+        <v>2000</v>
+      </c>
+      <c r="AU2" s="31">
+        <v>20</v>
+      </c>
+      <c r="AV2" s="31">
         <v>1620</v>
       </c>
-      <c r="AK2" s="31">
-        <v>20</v>
-      </c>
-      <c r="AL2" s="32">
+      <c r="AW2" s="31">
+        <v>20</v>
+      </c>
+      <c r="AX2" s="31">
         <v>1620</v>
       </c>
+      <c r="AY2" s="31">
+        <v>20</v>
+      </c>
+      <c r="AZ2" s="32">
+        <v>1620</v>
+      </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A3" s="36">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A3" s="17">
         <v>83</v>
       </c>
-      <c r="B3" s="37" t="s">
-        <v>30</v>
+      <c r="B3" s="42" t="s">
+        <v>28</v>
       </c>
       <c r="C3" s="37">
         <v>-15</v>
@@ -2677,34 +2799,34 @@
       <c r="J3" s="37">
         <v>2000</v>
       </c>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37">
-        <v>20</v>
-      </c>
-      <c r="N3" s="37">
-        <v>2000</v>
-      </c>
+      <c r="K3" s="37">
+        <v>20</v>
+      </c>
+      <c r="L3" s="37">
+        <v>2000</v>
+      </c>
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
       <c r="O3" s="37">
         <v>20</v>
       </c>
       <c r="P3" s="37">
         <v>2000</v>
       </c>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37"/>
+      <c r="Q3" s="37">
+        <v>20</v>
+      </c>
+      <c r="R3" s="37">
+        <v>2000</v>
+      </c>
       <c r="S3" s="37">
         <v>20</v>
       </c>
       <c r="T3" s="37">
         <v>2000</v>
       </c>
-      <c r="U3" s="37">
-        <v>20</v>
-      </c>
-      <c r="V3" s="37">
-        <v>2000</v>
-      </c>
+      <c r="U3" s="37"/>
+      <c r="V3" s="37"/>
       <c r="W3" s="37">
         <v>20</v>
       </c>
@@ -2745,21 +2867,63 @@
         <v>20</v>
       </c>
       <c r="AJ3" s="37">
+        <v>2000</v>
+      </c>
+      <c r="AK3" s="37">
+        <v>20</v>
+      </c>
+      <c r="AL3" s="37">
+        <v>2000</v>
+      </c>
+      <c r="AM3" s="37">
+        <v>20</v>
+      </c>
+      <c r="AN3" s="37">
+        <v>2000</v>
+      </c>
+      <c r="AO3" s="37">
+        <v>20</v>
+      </c>
+      <c r="AP3" s="37">
+        <v>2000</v>
+      </c>
+      <c r="AQ3" s="37">
+        <v>20</v>
+      </c>
+      <c r="AR3" s="37">
+        <v>2000</v>
+      </c>
+      <c r="AS3" s="37">
+        <v>20</v>
+      </c>
+      <c r="AT3" s="37">
+        <v>2000</v>
+      </c>
+      <c r="AU3" s="37">
+        <v>20</v>
+      </c>
+      <c r="AV3" s="37">
         <v>1620</v>
       </c>
-      <c r="AK3" s="37">
-        <v>20</v>
-      </c>
-      <c r="AL3" s="38">
+      <c r="AW3" s="37">
+        <v>20</v>
+      </c>
+      <c r="AX3" s="37">
         <v>1620</v>
       </c>
+      <c r="AY3" s="37">
+        <v>20</v>
+      </c>
+      <c r="AZ3" s="38">
+        <v>1620</v>
+      </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A4" s="30">
+    <row r="4" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
         <v>83</v>
       </c>
-      <c r="B4" s="31" t="s">
-        <v>31</v>
+      <c r="B4" s="10" t="s">
+        <v>29</v>
       </c>
       <c r="C4" s="31">
         <v>-65</v>
@@ -2781,34 +2945,34 @@
       <c r="J4" s="31">
         <v>2000</v>
       </c>
-      <c r="K4" s="31"/>
-      <c r="L4" s="31"/>
-      <c r="M4" s="31">
-        <v>20</v>
-      </c>
-      <c r="N4" s="31">
-        <v>2000</v>
-      </c>
+      <c r="K4" s="31">
+        <v>20</v>
+      </c>
+      <c r="L4" s="31">
+        <v>2000</v>
+      </c>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
       <c r="O4" s="31">
         <v>20</v>
       </c>
       <c r="P4" s="31">
         <v>2000</v>
       </c>
-      <c r="Q4" s="31"/>
-      <c r="R4" s="31"/>
+      <c r="Q4" s="31">
+        <v>20</v>
+      </c>
+      <c r="R4" s="31">
+        <v>2000</v>
+      </c>
       <c r="S4" s="31">
         <v>20</v>
       </c>
       <c r="T4" s="31">
         <v>2000</v>
       </c>
-      <c r="U4" s="31">
-        <v>20</v>
-      </c>
-      <c r="V4" s="31">
-        <v>2000</v>
-      </c>
+      <c r="U4" s="31"/>
+      <c r="V4" s="31"/>
       <c r="W4" s="31">
         <v>20</v>
       </c>
@@ -2849,21 +3013,63 @@
         <v>20</v>
       </c>
       <c r="AJ4" s="31">
+        <v>2000</v>
+      </c>
+      <c r="AK4" s="31">
+        <v>20</v>
+      </c>
+      <c r="AL4" s="31">
+        <v>2000</v>
+      </c>
+      <c r="AM4" s="31">
+        <v>20</v>
+      </c>
+      <c r="AN4" s="31">
+        <v>2000</v>
+      </c>
+      <c r="AO4" s="31">
+        <v>20</v>
+      </c>
+      <c r="AP4" s="31">
+        <v>2000</v>
+      </c>
+      <c r="AQ4" s="31">
+        <v>20</v>
+      </c>
+      <c r="AR4" s="31">
+        <v>2000</v>
+      </c>
+      <c r="AS4" s="31">
+        <v>20</v>
+      </c>
+      <c r="AT4" s="31">
+        <v>2000</v>
+      </c>
+      <c r="AU4" s="31">
+        <v>20</v>
+      </c>
+      <c r="AV4" s="31">
         <v>1620</v>
       </c>
-      <c r="AK4" s="31">
-        <v>20</v>
-      </c>
-      <c r="AL4" s="32">
+      <c r="AW4" s="31">
+        <v>20</v>
+      </c>
+      <c r="AX4" s="31">
         <v>1620</v>
       </c>
+      <c r="AY4" s="31">
+        <v>20</v>
+      </c>
+      <c r="AZ4" s="32">
+        <v>1620</v>
+      </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A5" s="36">
+    <row r="5" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A5" s="17">
         <v>83</v>
       </c>
-      <c r="B5" s="37" t="s">
-        <v>32</v>
+      <c r="B5" s="42" t="s">
+        <v>30</v>
       </c>
       <c r="C5" s="37">
         <v>0</v>
@@ -2885,34 +3091,34 @@
       <c r="J5" s="37">
         <v>2000</v>
       </c>
-      <c r="K5" s="37"/>
-      <c r="L5" s="37"/>
-      <c r="M5" s="37">
-        <v>20</v>
-      </c>
-      <c r="N5" s="37">
-        <v>2000</v>
-      </c>
+      <c r="K5" s="37">
+        <v>20</v>
+      </c>
+      <c r="L5" s="37">
+        <v>2000</v>
+      </c>
+      <c r="M5" s="37"/>
+      <c r="N5" s="37"/>
       <c r="O5" s="37">
         <v>20</v>
       </c>
       <c r="P5" s="37">
         <v>2000</v>
       </c>
-      <c r="Q5" s="37"/>
-      <c r="R5" s="37"/>
+      <c r="Q5" s="37">
+        <v>20</v>
+      </c>
+      <c r="R5" s="37">
+        <v>2000</v>
+      </c>
       <c r="S5" s="37">
         <v>20</v>
       </c>
       <c r="T5" s="37">
         <v>2000</v>
       </c>
-      <c r="U5" s="37">
-        <v>20</v>
-      </c>
-      <c r="V5" s="37">
-        <v>2000</v>
-      </c>
+      <c r="U5" s="37"/>
+      <c r="V5" s="37"/>
       <c r="W5" s="37">
         <v>20</v>
       </c>
@@ -2953,21 +3159,63 @@
         <v>20</v>
       </c>
       <c r="AJ5" s="37">
+        <v>2000</v>
+      </c>
+      <c r="AK5" s="37">
+        <v>20</v>
+      </c>
+      <c r="AL5" s="37">
+        <v>2000</v>
+      </c>
+      <c r="AM5" s="37">
+        <v>20</v>
+      </c>
+      <c r="AN5" s="37">
+        <v>2000</v>
+      </c>
+      <c r="AO5" s="37">
+        <v>20</v>
+      </c>
+      <c r="AP5" s="37">
+        <v>2000</v>
+      </c>
+      <c r="AQ5" s="37">
+        <v>20</v>
+      </c>
+      <c r="AR5" s="37">
+        <v>2000</v>
+      </c>
+      <c r="AS5" s="37">
+        <v>20</v>
+      </c>
+      <c r="AT5" s="37">
+        <v>2000</v>
+      </c>
+      <c r="AU5" s="37">
+        <v>20</v>
+      </c>
+      <c r="AV5" s="37">
         <v>1620</v>
       </c>
-      <c r="AK5" s="37">
-        <v>20</v>
-      </c>
-      <c r="AL5" s="38">
+      <c r="AW5" s="37">
+        <v>20</v>
+      </c>
+      <c r="AX5" s="37">
         <v>1620</v>
       </c>
+      <c r="AY5" s="37">
+        <v>20</v>
+      </c>
+      <c r="AZ5" s="38">
+        <v>1620</v>
+      </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A6" s="30">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
         <v>81</v>
       </c>
-      <c r="B6" s="31" t="s">
-        <v>33</v>
+      <c r="B6" s="10" t="s">
+        <v>31</v>
       </c>
       <c r="C6" s="31">
         <v>-423</v>
@@ -2989,51 +3237,51 @@
       <c r="J6" s="31">
         <v>1000</v>
       </c>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
-      <c r="M6" s="31">
+      <c r="K6" s="31">
         <v>50</v>
       </c>
-      <c r="N6" s="31">
-        <v>900</v>
-      </c>
+      <c r="L6" s="31">
+        <v>1000</v>
+      </c>
+      <c r="M6" s="31"/>
+      <c r="N6" s="31"/>
       <c r="O6" s="31">
         <v>50</v>
       </c>
       <c r="P6" s="31">
         <v>900</v>
       </c>
-      <c r="Q6" s="31"/>
-      <c r="R6" s="31"/>
+      <c r="Q6" s="31">
+        <v>50</v>
+      </c>
+      <c r="R6" s="31">
+        <v>900</v>
+      </c>
       <c r="S6" s="31">
         <v>50</v>
       </c>
       <c r="T6" s="31">
         <v>900</v>
       </c>
-      <c r="U6" s="31">
-        <v>50</v>
-      </c>
-      <c r="V6" s="31">
-        <v>900</v>
-      </c>
+      <c r="U6" s="31"/>
+      <c r="V6" s="31"/>
       <c r="W6" s="31">
         <v>50</v>
       </c>
       <c r="X6" s="31">
-        <v>500</v>
+        <v>900</v>
       </c>
       <c r="Y6" s="31">
         <v>50</v>
       </c>
       <c r="Z6" s="31">
-        <v>500</v>
+        <v>900</v>
       </c>
       <c r="AA6" s="31">
         <v>50</v>
       </c>
       <c r="AB6" s="31">
-        <v>500</v>
+        <v>900</v>
       </c>
       <c r="AC6" s="31">
         <v>50</v>
@@ -3062,16 +3310,58 @@
       <c r="AK6" s="31">
         <v>50</v>
       </c>
-      <c r="AL6" s="32">
+      <c r="AL6" s="31">
         <v>500</v>
       </c>
+      <c r="AM6" s="31">
+        <v>50</v>
+      </c>
+      <c r="AN6" s="31">
+        <v>500</v>
+      </c>
+      <c r="AO6" s="31">
+        <v>50</v>
+      </c>
+      <c r="AP6" s="31">
+        <v>500</v>
+      </c>
+      <c r="AQ6" s="31">
+        <v>50</v>
+      </c>
+      <c r="AR6" s="31">
+        <v>500</v>
+      </c>
+      <c r="AS6" s="31">
+        <v>50</v>
+      </c>
+      <c r="AT6" s="31">
+        <v>500</v>
+      </c>
+      <c r="AU6" s="31">
+        <v>50</v>
+      </c>
+      <c r="AV6" s="31">
+        <v>500</v>
+      </c>
+      <c r="AW6" s="31">
+        <v>50</v>
+      </c>
+      <c r="AX6" s="31">
+        <v>500</v>
+      </c>
+      <c r="AY6" s="31">
+        <v>50</v>
+      </c>
+      <c r="AZ6" s="32">
+        <v>500</v>
+      </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A7" s="36">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A7" s="17">
         <v>81</v>
       </c>
-      <c r="B7" s="37" t="s">
-        <v>34</v>
+      <c r="B7" s="42" t="s">
+        <v>32</v>
       </c>
       <c r="C7" s="37">
         <v>-423</v>
@@ -3093,51 +3383,51 @@
       <c r="J7" s="37">
         <v>4000</v>
       </c>
-      <c r="K7" s="37"/>
-      <c r="L7" s="37"/>
-      <c r="M7" s="37">
-        <v>901</v>
-      </c>
-      <c r="N7" s="37">
-        <v>1500</v>
-      </c>
+      <c r="K7" s="37">
+        <v>1001</v>
+      </c>
+      <c r="L7" s="37">
+        <v>4000</v>
+      </c>
+      <c r="M7" s="37"/>
+      <c r="N7" s="37"/>
       <c r="O7" s="37">
         <v>901</v>
       </c>
       <c r="P7" s="37">
         <v>1500</v>
       </c>
-      <c r="Q7" s="37"/>
-      <c r="R7" s="37"/>
+      <c r="Q7" s="37">
+        <v>901</v>
+      </c>
+      <c r="R7" s="37">
+        <v>1500</v>
+      </c>
       <c r="S7" s="37">
         <v>901</v>
       </c>
       <c r="T7" s="37">
         <v>1500</v>
       </c>
-      <c r="U7" s="37">
+      <c r="U7" s="37"/>
+      <c r="V7" s="37"/>
+      <c r="W7" s="37">
         <v>901</v>
       </c>
-      <c r="V7" s="37">
+      <c r="X7" s="37">
         <v>1500</v>
       </c>
-      <c r="W7" s="37">
-        <v>501</v>
-      </c>
-      <c r="X7" s="37">
-        <v>750</v>
-      </c>
       <c r="Y7" s="37">
-        <v>501</v>
+        <v>901</v>
       </c>
       <c r="Z7" s="37">
-        <v>750</v>
+        <v>1500</v>
       </c>
       <c r="AA7" s="37">
-        <v>501</v>
+        <v>901</v>
       </c>
       <c r="AB7" s="37">
-        <v>750</v>
+        <v>1500</v>
       </c>
       <c r="AC7" s="37">
         <v>501</v>
@@ -3166,16 +3456,58 @@
       <c r="AK7" s="37">
         <v>501</v>
       </c>
-      <c r="AL7" s="38">
+      <c r="AL7" s="37">
         <v>750</v>
       </c>
+      <c r="AM7" s="37">
+        <v>501</v>
+      </c>
+      <c r="AN7" s="37">
+        <v>750</v>
+      </c>
+      <c r="AO7" s="37">
+        <v>501</v>
+      </c>
+      <c r="AP7" s="37">
+        <v>750</v>
+      </c>
+      <c r="AQ7" s="37">
+        <v>501</v>
+      </c>
+      <c r="AR7" s="37">
+        <v>750</v>
+      </c>
+      <c r="AS7" s="37">
+        <v>501</v>
+      </c>
+      <c r="AT7" s="37">
+        <v>750</v>
+      </c>
+      <c r="AU7" s="37">
+        <v>501</v>
+      </c>
+      <c r="AV7" s="37">
+        <v>750</v>
+      </c>
+      <c r="AW7" s="37">
+        <v>501</v>
+      </c>
+      <c r="AX7" s="37">
+        <v>750</v>
+      </c>
+      <c r="AY7" s="37">
+        <v>501</v>
+      </c>
+      <c r="AZ7" s="38">
+        <v>750</v>
+      </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A8" s="30">
+    <row r="8" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
         <v>81</v>
       </c>
-      <c r="B8" s="31" t="s">
-        <v>35</v>
+      <c r="B8" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="C8" s="31">
         <v>-423</v>
@@ -3193,89 +3525,131 @@
       <c r="J8" s="31">
         <v>10000</v>
       </c>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="31">
-        <v>1501</v>
-      </c>
-      <c r="N8" s="31">
-        <v>9600</v>
-      </c>
+      <c r="K8" s="31">
+        <v>4001</v>
+      </c>
+      <c r="L8" s="31">
+        <v>10000</v>
+      </c>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
       <c r="O8" s="31">
         <v>1501</v>
       </c>
       <c r="P8" s="31">
         <v>9600</v>
       </c>
-      <c r="Q8" s="31"/>
-      <c r="R8" s="31"/>
+      <c r="Q8" s="31">
+        <v>1501</v>
+      </c>
+      <c r="R8" s="31">
+        <v>9600</v>
+      </c>
       <c r="S8" s="31">
         <v>1501</v>
       </c>
       <c r="T8" s="31">
+        <v>9600</v>
+      </c>
+      <c r="U8" s="31"/>
+      <c r="V8" s="31"/>
+      <c r="W8" s="31">
+        <v>1501</v>
+      </c>
+      <c r="X8" s="31">
         <v>4000</v>
       </c>
-      <c r="U8" s="31">
+      <c r="Y8" s="31">
         <v>1501</v>
       </c>
-      <c r="V8" s="31">
+      <c r="Z8" s="31">
         <v>4000</v>
       </c>
-      <c r="W8" s="31">
-        <v>751</v>
-      </c>
-      <c r="X8" s="31">
-        <v>2990</v>
-      </c>
-      <c r="Y8" s="31">
-        <v>751</v>
-      </c>
-      <c r="Z8" s="31">
-        <v>4040</v>
-      </c>
       <c r="AA8" s="31">
-        <v>752</v>
+        <v>1501</v>
       </c>
       <c r="AB8" s="31">
-        <v>2750</v>
+        <v>4000</v>
       </c>
       <c r="AC8" s="31">
         <v>751</v>
       </c>
       <c r="AD8" s="31">
-        <v>2570</v>
+        <v>2990</v>
       </c>
       <c r="AE8" s="31">
         <v>751</v>
       </c>
       <c r="AF8" s="31">
-        <v>2270</v>
+        <v>4040</v>
       </c>
       <c r="AG8" s="31">
         <v>751</v>
       </c>
       <c r="AH8" s="31">
-        <v>2580</v>
+        <v>4040</v>
       </c>
       <c r="AI8" s="31">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="AJ8" s="31">
-        <v>1620</v>
+        <v>2750</v>
       </c>
       <c r="AK8" s="31">
         <v>751</v>
       </c>
-      <c r="AL8" s="32">
+      <c r="AL8" s="31">
+        <v>2570</v>
+      </c>
+      <c r="AM8" s="31">
+        <v>751</v>
+      </c>
+      <c r="AN8" s="31">
+        <v>2570</v>
+      </c>
+      <c r="AO8" s="31">
+        <v>751</v>
+      </c>
+      <c r="AP8" s="31">
+        <v>2270</v>
+      </c>
+      <c r="AQ8" s="31">
+        <v>751</v>
+      </c>
+      <c r="AR8" s="31">
+        <v>2580</v>
+      </c>
+      <c r="AS8" s="31">
+        <v>751</v>
+      </c>
+      <c r="AT8" s="31">
+        <v>2580</v>
+      </c>
+      <c r="AU8" s="31">
+        <v>751</v>
+      </c>
+      <c r="AV8" s="31">
         <v>1620</v>
       </c>
+      <c r="AW8" s="31">
+        <v>751</v>
+      </c>
+      <c r="AX8" s="31">
+        <v>1620</v>
+      </c>
+      <c r="AY8" s="31">
+        <v>751</v>
+      </c>
+      <c r="AZ8" s="32">
+        <v>1620</v>
+      </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A9" s="36" t="s">
+    <row r="9" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="37" t="s">
-        <v>33</v>
+      <c r="B9" s="42" t="s">
+        <v>31</v>
       </c>
       <c r="C9" s="37">
         <v>-65</v>
@@ -3297,42 +3671,42 @@
       <c r="J9" s="37">
         <v>2000</v>
       </c>
-      <c r="K9" s="37"/>
-      <c r="L9" s="37"/>
+      <c r="K9" s="37">
+        <v>50</v>
+      </c>
+      <c r="L9" s="37">
+        <v>2000</v>
+      </c>
       <c r="M9" s="37"/>
       <c r="N9" s="37"/>
       <c r="O9" s="37"/>
       <c r="P9" s="37"/>
       <c r="Q9" s="37"/>
       <c r="R9" s="37"/>
-      <c r="S9" s="37">
+      <c r="S9" s="37"/>
+      <c r="T9" s="37"/>
+      <c r="U9" s="37"/>
+      <c r="V9" s="37"/>
+      <c r="W9" s="37">
         <v>50</v>
       </c>
-      <c r="T9" s="37">
-        <v>2000</v>
-      </c>
-      <c r="U9" s="37">
+      <c r="X9" s="37">
+        <v>2000</v>
+      </c>
+      <c r="Y9" s="37">
         <v>50</v>
       </c>
-      <c r="V9" s="37">
-        <v>2000</v>
-      </c>
-      <c r="W9" s="37"/>
-      <c r="X9" s="37"/>
-      <c r="Y9" s="37"/>
-      <c r="Z9" s="37"/>
+      <c r="Z9" s="37">
+        <v>2000</v>
+      </c>
       <c r="AA9" s="37">
         <v>50</v>
       </c>
       <c r="AB9" s="37">
-        <v>1000</v>
-      </c>
-      <c r="AC9" s="37">
-        <v>50</v>
-      </c>
-      <c r="AD9" s="37">
-        <v>1000</v>
-      </c>
+        <v>2000</v>
+      </c>
+      <c r="AC9" s="37"/>
+      <c r="AD9" s="37"/>
       <c r="AE9" s="37"/>
       <c r="AF9" s="37"/>
       <c r="AG9" s="37"/>
@@ -3346,16 +3720,46 @@
       <c r="AK9" s="37">
         <v>50</v>
       </c>
-      <c r="AL9" s="38">
+      <c r="AL9" s="37">
         <v>1000</v>
       </c>
+      <c r="AM9" s="37">
+        <v>50</v>
+      </c>
+      <c r="AN9" s="37">
+        <v>1000</v>
+      </c>
+      <c r="AO9" s="37"/>
+      <c r="AP9" s="37"/>
+      <c r="AQ9" s="37"/>
+      <c r="AR9" s="37"/>
+      <c r="AS9" s="37"/>
+      <c r="AT9" s="37"/>
+      <c r="AU9" s="37">
+        <v>50</v>
+      </c>
+      <c r="AV9" s="37">
+        <v>1000</v>
+      </c>
+      <c r="AW9" s="37">
+        <v>50</v>
+      </c>
+      <c r="AX9" s="37">
+        <v>1000</v>
+      </c>
+      <c r="AY9" s="37">
+        <v>50</v>
+      </c>
+      <c r="AZ9" s="38">
+        <v>1000</v>
+      </c>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A10" s="30" t="s">
+    <row r="10" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="31" t="s">
-        <v>34</v>
+      <c r="B10" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="C10" s="31">
         <v>-65</v>
@@ -3377,42 +3781,42 @@
       <c r="J10" s="31">
         <v>6000</v>
       </c>
-      <c r="K10" s="31"/>
-      <c r="L10" s="31"/>
+      <c r="K10" s="31">
+        <v>2001</v>
+      </c>
+      <c r="L10" s="31">
+        <v>6000</v>
+      </c>
       <c r="M10" s="31"/>
       <c r="N10" s="31"/>
       <c r="O10" s="31"/>
       <c r="P10" s="31"/>
       <c r="Q10" s="31"/>
       <c r="R10" s="31"/>
-      <c r="S10" s="31">
+      <c r="S10" s="31"/>
+      <c r="T10" s="31"/>
+      <c r="U10" s="31"/>
+      <c r="V10" s="31"/>
+      <c r="W10" s="31">
         <v>2001</v>
       </c>
-      <c r="T10" s="31">
+      <c r="X10" s="31">
         <v>4000</v>
       </c>
-      <c r="U10" s="31">
+      <c r="Y10" s="31">
         <v>2001</v>
       </c>
-      <c r="V10" s="31">
+      <c r="Z10" s="31">
         <v>4000</v>
       </c>
-      <c r="W10" s="31"/>
-      <c r="X10" s="31"/>
-      <c r="Y10" s="31"/>
-      <c r="Z10" s="31"/>
       <c r="AA10" s="31">
-        <v>1001</v>
+        <v>2001</v>
       </c>
       <c r="AB10" s="31">
-        <v>2570</v>
-      </c>
-      <c r="AC10" s="31">
-        <v>1001</v>
-      </c>
-      <c r="AD10" s="31">
-        <v>6000</v>
-      </c>
+        <v>4000</v>
+      </c>
+      <c r="AC10" s="31"/>
+      <c r="AD10" s="31"/>
       <c r="AE10" s="31"/>
       <c r="AF10" s="31"/>
       <c r="AG10" s="31"/>
@@ -3421,21 +3825,51 @@
         <v>1001</v>
       </c>
       <c r="AJ10" s="31">
-        <v>1620</v>
+        <v>2570</v>
       </c>
       <c r="AK10" s="31">
         <v>1001</v>
       </c>
-      <c r="AL10" s="32">
+      <c r="AL10" s="31">
+        <v>6000</v>
+      </c>
+      <c r="AM10" s="31">
+        <v>1001</v>
+      </c>
+      <c r="AN10" s="31">
+        <v>6000</v>
+      </c>
+      <c r="AO10" s="31"/>
+      <c r="AP10" s="31"/>
+      <c r="AQ10" s="31"/>
+      <c r="AR10" s="31"/>
+      <c r="AS10" s="31"/>
+      <c r="AT10" s="31"/>
+      <c r="AU10" s="31">
+        <v>1001</v>
+      </c>
+      <c r="AV10" s="31">
         <v>1620</v>
       </c>
+      <c r="AW10" s="31">
+        <v>1001</v>
+      </c>
+      <c r="AX10" s="31">
+        <v>1620</v>
+      </c>
+      <c r="AY10" s="31">
+        <v>1001</v>
+      </c>
+      <c r="AZ10" s="32">
+        <v>1620</v>
+      </c>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A11" s="36">
+    <row r="11" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A11" s="17">
         <v>84</v>
       </c>
-      <c r="B11" s="37" t="s">
-        <v>39</v>
+      <c r="B11" s="42" t="s">
+        <v>36</v>
       </c>
       <c r="C11" s="37">
         <v>-40</v>
@@ -3480,14 +3914,28 @@
       <c r="AI11" s="37"/>
       <c r="AJ11" s="37"/>
       <c r="AK11" s="37"/>
-      <c r="AL11" s="38"/>
+      <c r="AL11" s="37"/>
+      <c r="AM11" s="37"/>
+      <c r="AN11" s="37"/>
+      <c r="AO11" s="37"/>
+      <c r="AP11" s="37"/>
+      <c r="AQ11" s="37"/>
+      <c r="AR11" s="37"/>
+      <c r="AS11" s="37"/>
+      <c r="AT11" s="37"/>
+      <c r="AU11" s="37"/>
+      <c r="AV11" s="37"/>
+      <c r="AW11" s="37"/>
+      <c r="AX11" s="37"/>
+      <c r="AY11" s="37"/>
+      <c r="AZ11" s="38"/>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A12" s="30" t="s">
+    <row r="12" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="31" t="s">
-        <v>26</v>
+      <c r="B12" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="C12" s="31">
         <v>-65</v>
@@ -3501,26 +3949,26 @@
       <c r="H12" s="31"/>
       <c r="I12" s="31"/>
       <c r="J12" s="31"/>
-      <c r="K12" s="31">
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31">
         <v>37</v>
       </c>
-      <c r="L12" s="31">
+      <c r="N12" s="31">
         <v>531</v>
       </c>
-      <c r="M12" s="31"/>
-      <c r="N12" s="31"/>
       <c r="O12" s="31"/>
       <c r="P12" s="31"/>
-      <c r="Q12" s="31">
-        <v>45</v>
-      </c>
-      <c r="R12" s="31">
-        <v>374</v>
-      </c>
+      <c r="Q12" s="31"/>
+      <c r="R12" s="31"/>
       <c r="S12" s="31"/>
       <c r="T12" s="31"/>
-      <c r="U12" s="31"/>
-      <c r="V12" s="31"/>
+      <c r="U12" s="31">
+        <v>45</v>
+      </c>
+      <c r="V12" s="31">
+        <v>374</v>
+      </c>
       <c r="W12" s="31"/>
       <c r="X12" s="31"/>
       <c r="Y12" s="31"/>
@@ -3536,14 +3984,28 @@
       <c r="AI12" s="31"/>
       <c r="AJ12" s="31"/>
       <c r="AK12" s="31"/>
-      <c r="AL12" s="32"/>
+      <c r="AL12" s="31"/>
+      <c r="AM12" s="31"/>
+      <c r="AN12" s="31"/>
+      <c r="AO12" s="31"/>
+      <c r="AP12" s="31"/>
+      <c r="AQ12" s="31"/>
+      <c r="AR12" s="31"/>
+      <c r="AS12" s="31"/>
+      <c r="AT12" s="31"/>
+      <c r="AU12" s="31"/>
+      <c r="AV12" s="31"/>
+      <c r="AW12" s="31"/>
+      <c r="AX12" s="31"/>
+      <c r="AY12" s="31"/>
+      <c r="AZ12" s="32"/>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A13" s="36" t="s">
+    <row r="13" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="37" t="s">
-        <v>30</v>
+      <c r="B13" s="42" t="s">
+        <v>28</v>
       </c>
       <c r="C13" s="37">
         <v>-15</v>
@@ -3557,26 +4019,26 @@
       <c r="H13" s="37"/>
       <c r="I13" s="37"/>
       <c r="J13" s="37"/>
-      <c r="K13" s="37">
+      <c r="K13" s="37"/>
+      <c r="L13" s="37"/>
+      <c r="M13" s="37">
         <v>37</v>
       </c>
-      <c r="L13" s="37">
+      <c r="N13" s="37">
         <v>531</v>
       </c>
-      <c r="M13" s="37"/>
-      <c r="N13" s="37"/>
       <c r="O13" s="37"/>
       <c r="P13" s="37"/>
-      <c r="Q13" s="37">
-        <v>45</v>
-      </c>
-      <c r="R13" s="37">
-        <v>374</v>
-      </c>
+      <c r="Q13" s="37"/>
+      <c r="R13" s="37"/>
       <c r="S13" s="37"/>
       <c r="T13" s="37"/>
-      <c r="U13" s="37"/>
-      <c r="V13" s="37"/>
+      <c r="U13" s="37">
+        <v>45</v>
+      </c>
+      <c r="V13" s="37">
+        <v>374</v>
+      </c>
       <c r="W13" s="37"/>
       <c r="X13" s="37"/>
       <c r="Y13" s="37"/>
@@ -3592,14 +4054,28 @@
       <c r="AI13" s="37"/>
       <c r="AJ13" s="37"/>
       <c r="AK13" s="37"/>
-      <c r="AL13" s="38"/>
+      <c r="AL13" s="37"/>
+      <c r="AM13" s="37"/>
+      <c r="AN13" s="37"/>
+      <c r="AO13" s="37"/>
+      <c r="AP13" s="37"/>
+      <c r="AQ13" s="37"/>
+      <c r="AR13" s="37"/>
+      <c r="AS13" s="37"/>
+      <c r="AT13" s="37"/>
+      <c r="AU13" s="37"/>
+      <c r="AV13" s="37"/>
+      <c r="AW13" s="37"/>
+      <c r="AX13" s="37"/>
+      <c r="AY13" s="37"/>
+      <c r="AZ13" s="38"/>
     </row>
-    <row r="14" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="33" t="s">
+    <row r="14" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="34" t="s">
-        <v>31</v>
+      <c r="B14" s="43" t="s">
+        <v>29</v>
       </c>
       <c r="C14" s="34">
         <v>-65</v>
@@ -3613,26 +4089,26 @@
       <c r="H14" s="34"/>
       <c r="I14" s="34"/>
       <c r="J14" s="34"/>
-      <c r="K14" s="34">
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34">
         <v>371</v>
       </c>
-      <c r="L14" s="34">
+      <c r="N14" s="34">
         <v>531</v>
       </c>
-      <c r="M14" s="34"/>
-      <c r="N14" s="34"/>
       <c r="O14" s="34"/>
       <c r="P14" s="34"/>
-      <c r="Q14" s="34">
-        <v>45</v>
-      </c>
-      <c r="R14" s="34">
-        <v>374</v>
-      </c>
+      <c r="Q14" s="34"/>
+      <c r="R14" s="34"/>
       <c r="S14" s="34"/>
       <c r="T14" s="34"/>
-      <c r="U14" s="34"/>
-      <c r="V14" s="34"/>
+      <c r="U14" s="34">
+        <v>45</v>
+      </c>
+      <c r="V14" s="34">
+        <v>374</v>
+      </c>
       <c r="W14" s="34"/>
       <c r="X14" s="34"/>
       <c r="Y14" s="34"/>
@@ -3648,12 +4124,21 @@
       <c r="AI14" s="34"/>
       <c r="AJ14" s="34"/>
       <c r="AK14" s="34"/>
-      <c r="AL14" s="35"/>
-    </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="I15" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="AL14" s="34"/>
+      <c r="AM14" s="34"/>
+      <c r="AN14" s="34"/>
+      <c r="AO14" s="34"/>
+      <c r="AP14" s="34"/>
+      <c r="AQ14" s="34"/>
+      <c r="AR14" s="34"/>
+      <c r="AS14" s="34"/>
+      <c r="AT14" s="34"/>
+      <c r="AU14" s="34"/>
+      <c r="AV14" s="34"/>
+      <c r="AW14" s="34"/>
+      <c r="AX14" s="34"/>
+      <c r="AY14" s="34"/>
+      <c r="AZ14" s="35"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3675,7 +4160,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" s="26" t="s">
         <v>20</v>
@@ -3686,7 +4171,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B2" s="31">
         <v>-325</v>
@@ -3697,7 +4182,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B3" s="37">
         <v>-20</v>
@@ -3708,90 +4193,13 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="34">
         <v>-423</v>
       </c>
       <c r="C4" s="35">
         <v>550</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D368A94-4BF2-45ED-863C-19D230F439F9}">
-  <dimension ref="A1:K4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>